<commit_message>
improved usability, added helpbox
</commit_message>
<xml_diff>
--- a/trends.xlsx
+++ b/trends.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mmi/workspaces/shub/symbioticon-2019-slot-machine/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C2C5F3B-9B2B-2449-A29F-88B999274952}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDD92C20-BE8B-3C42-AB2A-9D45E0C9515E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18680" xr2:uid="{B6AAB51A-975A-FF42-AF23-E449566C1E86}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="31260" windowHeight="20540" activeTab="1" xr2:uid="{B6AAB51A-975A-FF42-AF23-E449566C1E86}"/>
   </bookViews>
   <sheets>
     <sheet name="trends" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="159">
   <si>
     <t>Wissenskultur</t>
   </si>
@@ -440,7 +440,76 @@
     <t>Simplexity</t>
   </si>
   <si>
-    <t>konn.png</t>
+    <t>Konnektivität.svg</t>
+  </si>
+  <si>
+    <t>Gender Shift.svg</t>
+  </si>
+  <si>
+    <t>Gesundheit.svg</t>
+  </si>
+  <si>
+    <t>Globalisierung.svg</t>
+  </si>
+  <si>
+    <t>Individualisierung.svg</t>
+  </si>
+  <si>
+    <t>Mobilität.svg</t>
+  </si>
+  <si>
+    <t>Neo-Ökologie.svg</t>
+  </si>
+  <si>
+    <t>New Work.svg</t>
+  </si>
+  <si>
+    <t>Sicherheit.svg</t>
+  </si>
+  <si>
+    <t>Silver Society.svg</t>
+  </si>
+  <si>
+    <t>Urbanisierung.svg</t>
+  </si>
+  <si>
+    <t>Wissenskultur.svg</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>ö</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>t</t>
   </si>
 </sst>
 </file>
@@ -792,16 +861,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC721A76-31B5-5942-83B2-FF5724A5D504}">
-  <dimension ref="A1:L25"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.1640625" customWidth="1"/>
     <col min="2" max="2" width="22.5" customWidth="1"/>
+    <col min="9" max="9" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
@@ -844,616 +914,654 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="B2" t="s">
         <v>135</v>
       </c>
       <c r="C2" t="s">
-        <v>135</v>
+        <v>145</v>
       </c>
       <c r="D2" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="E2" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="F2" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="G2" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="H2" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="I2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="J2" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="K2" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="L2" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>147</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>148</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>149</v>
       </c>
       <c r="D3" t="s">
-        <v>48</v>
+        <v>154</v>
       </c>
       <c r="E3" t="s">
-        <v>61</v>
+        <v>157</v>
       </c>
       <c r="F3" t="s">
-        <v>71</v>
+        <v>152</v>
       </c>
       <c r="G3" t="s">
-        <v>81</v>
+        <v>153</v>
       </c>
       <c r="H3" t="s">
-        <v>92</v>
+        <v>150</v>
       </c>
       <c r="I3" t="s">
-        <v>106</v>
+        <v>158</v>
       </c>
       <c r="J3" t="s">
-        <v>114</v>
+        <v>151</v>
       </c>
       <c r="K3" t="s">
-        <v>119</v>
+        <v>156</v>
       </c>
       <c r="L3" t="s">
-        <v>130</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="L4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E5" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="F5" t="s">
-        <v>24</v>
+        <v>72</v>
       </c>
       <c r="G5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E6" t="s">
-        <v>63</v>
+        <v>22</v>
       </c>
       <c r="F6" t="s">
-        <v>73</v>
+        <v>24</v>
       </c>
       <c r="G6" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="H6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J6" t="s">
-        <v>25</v>
+        <v>116</v>
       </c>
       <c r="K6" t="s">
-        <v>34</v>
+        <v>121</v>
       </c>
       <c r="L6" t="s">
-        <v>25</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F7" t="s">
-        <v>26</v>
+        <v>73</v>
       </c>
       <c r="G7" t="s">
-        <v>24</v>
+        <v>72</v>
       </c>
       <c r="H7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I7" t="s">
-        <v>85</v>
+        <v>109</v>
       </c>
       <c r="J7" t="s">
-        <v>84</v>
+        <v>25</v>
       </c>
       <c r="K7" t="s">
-        <v>103</v>
+        <v>34</v>
       </c>
       <c r="L7" t="s">
-        <v>73</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F8" t="s">
-        <v>74</v>
+        <v>26</v>
       </c>
       <c r="G8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I8" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="J8" t="s">
-        <v>52</v>
+        <v>84</v>
       </c>
       <c r="K8" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="L8" t="s">
-        <v>133</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D9" t="s">
-        <v>10</v>
+        <v>53</v>
       </c>
       <c r="E9" t="s">
-        <v>27</v>
+        <v>65</v>
       </c>
       <c r="F9" t="s">
-        <v>53</v>
+        <v>74</v>
       </c>
       <c r="G9" t="s">
-        <v>84</v>
+        <v>25</v>
       </c>
       <c r="H9" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="I9" t="s">
-        <v>11</v>
+        <v>75</v>
       </c>
       <c r="J9" t="s">
-        <v>75</v>
+        <v>52</v>
       </c>
       <c r="K9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L9" t="s">
-        <v>6</v>
+        <v>133</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D10" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="E10" t="s">
-        <v>56</v>
+        <v>27</v>
       </c>
       <c r="F10" t="s">
+        <v>53</v>
+      </c>
+      <c r="G10" t="s">
+        <v>84</v>
+      </c>
+      <c r="H10" t="s">
+        <v>86</v>
+      </c>
+      <c r="I10" t="s">
+        <v>11</v>
+      </c>
+      <c r="J10" t="s">
         <v>75</v>
       </c>
-      <c r="G10" t="s">
-        <v>52</v>
-      </c>
-      <c r="H10" t="s">
-        <v>98</v>
-      </c>
-      <c r="I10" t="s">
-        <v>66</v>
-      </c>
-      <c r="J10" t="s">
-        <v>76</v>
-      </c>
       <c r="K10" t="s">
-        <v>39</v>
+        <v>123</v>
       </c>
       <c r="L10" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E11" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F11" t="s">
+        <v>75</v>
+      </c>
+      <c r="G11" t="s">
+        <v>52</v>
+      </c>
+      <c r="H11" t="s">
+        <v>98</v>
+      </c>
+      <c r="I11" t="s">
+        <v>66</v>
+      </c>
+      <c r="J11" t="s">
         <v>76</v>
       </c>
-      <c r="G11" t="s">
-        <v>85</v>
-      </c>
-      <c r="H11" t="s">
-        <v>75</v>
-      </c>
-      <c r="I11" t="s">
-        <v>110</v>
-      </c>
-      <c r="J11" t="s">
-        <v>97</v>
-      </c>
       <c r="K11" t="s">
-        <v>124</v>
+        <v>39</v>
       </c>
       <c r="L11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E12" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H12" t="s">
-        <v>11</v>
+        <v>75</v>
       </c>
       <c r="I12" t="s">
-        <v>78</v>
+        <v>110</v>
       </c>
       <c r="J12" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="K12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L12" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" t="s">
+        <v>56</v>
+      </c>
+      <c r="E13" t="s">
+        <v>54</v>
+      </c>
+      <c r="F13" t="s">
+        <v>77</v>
+      </c>
+      <c r="G13" t="s">
+        <v>86</v>
+      </c>
+      <c r="H13" t="s">
         <v>11</v>
       </c>
-      <c r="B13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" t="s">
-        <v>43</v>
-      </c>
-      <c r="D13" t="s">
-        <v>28</v>
-      </c>
-      <c r="E13" t="s">
-        <v>66</v>
-      </c>
-      <c r="F13" t="s">
-        <v>13</v>
-      </c>
-      <c r="G13" t="s">
+      <c r="I13" t="s">
+        <v>78</v>
+      </c>
+      <c r="J13" t="s">
         <v>87</v>
       </c>
-      <c r="H13" t="s">
-        <v>66</v>
-      </c>
-      <c r="I13" t="s">
-        <v>111</v>
-      </c>
-      <c r="J13" t="s">
-        <v>117</v>
-      </c>
       <c r="K13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D14" t="s">
-        <v>57</v>
+        <v>28</v>
       </c>
       <c r="E14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F14" t="s">
-        <v>78</v>
+        <v>13</v>
       </c>
       <c r="G14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H14" t="s">
-        <v>99</v>
+        <v>66</v>
       </c>
       <c r="I14" t="s">
-        <v>112</v>
+        <v>111</v>
+      </c>
+      <c r="J14" t="s">
+        <v>117</v>
       </c>
       <c r="K14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="L14" t="s">
-        <v>101</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="C15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H15" t="s">
-        <v>100</v>
+        <v>99</v>
+      </c>
+      <c r="I15" t="s">
+        <v>112</v>
       </c>
       <c r="K15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" t="s">
+        <v>68</v>
+      </c>
+      <c r="F16" t="s">
+        <v>79</v>
+      </c>
+      <c r="G16" t="s">
+        <v>89</v>
+      </c>
+      <c r="H16" t="s">
+        <v>100</v>
+      </c>
+      <c r="K16" t="s">
+        <v>128</v>
+      </c>
+      <c r="L16" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>14</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>27</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D17" t="s">
         <v>38</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E17" t="s">
         <v>42</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G17" t="s">
         <v>90</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H17" t="s">
         <v>55</v>
       </c>
-      <c r="L16" t="s">
+      <c r="L17" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>15</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>28</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D18" t="s">
         <v>39</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E18" t="s">
         <v>69</v>
       </c>
-      <c r="H17" t="s">
+      <c r="H18" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B18" t="s">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
         <v>29</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D19" t="s">
         <v>59</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B19" t="s">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
         <v>30</v>
       </c>
-      <c r="H19" t="s">
+      <c r="H20" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B20" t="s">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
         <v>31</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H21" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="H21" t="s">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H22" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="H22" t="s">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H23" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="H23" t="s">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H24" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="H24" t="s">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H25" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="H25" t="s">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H26" t="s">
         <v>104</v>
       </c>
     </row>
@@ -1466,8 +1574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{500DDF2F-334E-8A4E-AA45-571C0E2C5A60}">
   <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1541,51 +1649,51 @@
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
         <f>IF(ISBLANK(trends!A2),"","'"&amp;trends!A2&amp;"',")</f>
-        <v>'konn.png',</v>
+        <v>'Wissenskultur.svg',</v>
       </c>
       <c r="B2" t="str">
         <f>IF(ISBLANK(trends!B2),"","'"&amp;trends!B2&amp;"',")</f>
-        <v>'konn.png',</v>
+        <v>'Konnektivität.svg',</v>
       </c>
       <c r="C2" t="str">
         <f>IF(ISBLANK(trends!C2),"","'"&amp;trends!C2&amp;"',")</f>
-        <v>'konn.png',</v>
+        <v>'Urbanisierung.svg',</v>
       </c>
       <c r="D2" t="str">
         <f>IF(ISBLANK(trends!D2),"","'"&amp;trends!D2&amp;"',")</f>
-        <v>'konn.png',</v>
+        <v>'Neo-Ökologie.svg',</v>
       </c>
       <c r="E2" t="str">
         <f>IF(ISBLANK(trends!E2),"","'"&amp;trends!E2&amp;"',")</f>
-        <v>'konn.png',</v>
+        <v>'Globalisierung.svg',</v>
       </c>
       <c r="F2" t="str">
         <f>IF(ISBLANK(trends!F2),"","'"&amp;trends!F2&amp;"',")</f>
-        <v>'konn.png',</v>
+        <v>'Individualisierung.svg',</v>
       </c>
       <c r="G2" t="str">
         <f>IF(ISBLANK(trends!G2),"","'"&amp;trends!G2&amp;"',")</f>
-        <v>'konn.png',</v>
+        <v>'Gesundheit.svg',</v>
       </c>
       <c r="H2" t="str">
         <f>IF(ISBLANK(trends!H2),"","'"&amp;trends!H2&amp;"',")</f>
-        <v>'konn.png',</v>
+        <v>'New Work.svg',</v>
       </c>
       <c r="I2" t="str">
         <f>IF(ISBLANK(trends!I2),"","'"&amp;trends!I2&amp;"',")</f>
-        <v>'konn.png',</v>
+        <v>'Gender Shift.svg',</v>
       </c>
       <c r="J2" t="str">
         <f>IF(ISBLANK(trends!J2),"","'"&amp;trends!J2&amp;"',")</f>
-        <v>'konn.png',</v>
+        <v>'Silver Society.svg',</v>
       </c>
       <c r="K2" t="str">
         <f>IF(ISBLANK(trends!K2),"","'"&amp;trends!K2&amp;"',")</f>
-        <v>'konn.png',</v>
+        <v>'Mobilität.svg',</v>
       </c>
       <c r="L2" t="str">
         <f>IF(ISBLANK(trends!L2),"","'"&amp;trends!L2&amp;"',")</f>
-        <v>'konn.png',</v>
+        <v>'Sicherheit.svg',</v>
       </c>
       <c r="M2" t="str">
         <f>IF(ISBLANK(trends!M2),"","'"&amp;trends!M2&amp;"',")</f>
@@ -1607,51 +1715,51 @@
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
         <f>IF(ISBLANK(trends!A3),"","'"&amp;trends!A3&amp;"',")</f>
-        <v>'Open Science',</v>
+        <v>'w',</v>
       </c>
       <c r="B3" t="str">
         <f>IF(ISBLANK(trends!B3),"","'"&amp;trends!B3&amp;"',")</f>
-        <v>'Augmented Reality',</v>
+        <v>'k',</v>
       </c>
       <c r="C3" t="str">
         <f>IF(ISBLANK(trends!C3),"","'"&amp;trends!C3&amp;"',")</f>
-        <v>'Bevölkerungswachstum',</v>
+        <v>'u',</v>
       </c>
       <c r="D3" t="str">
         <f>IF(ISBLANK(trends!D3),"","'"&amp;trends!D3&amp;"',")</f>
-        <v>'Nachhaltigkeitsgesellschaft',</v>
+        <v>'ö',</v>
       </c>
       <c r="E3" t="str">
         <f>IF(ISBLANK(trends!E3),"","'"&amp;trends!E3&amp;"',")</f>
-        <v>'Glokalisierung',</v>
+        <v>'q',</v>
       </c>
       <c r="F3" t="str">
         <f>IF(ISBLANK(trends!F3),"","'"&amp;trends!F3&amp;"',")</f>
-        <v>'Single-Gesellschaft',</v>
+        <v>'i',</v>
       </c>
       <c r="G3" t="str">
         <f>IF(ISBLANK(trends!G3),"","'"&amp;trends!G3&amp;"',")</f>
-        <v>'Sportivity',</v>
+        <v>'g',</v>
       </c>
       <c r="H3" t="str">
         <f>IF(ISBLANK(trends!H3),"","'"&amp;trends!H3&amp;"',")</f>
-        <v>'Work-Design',</v>
+        <v>'n',</v>
       </c>
       <c r="I3" t="str">
         <f>IF(ISBLANK(trends!I3),"","'"&amp;trends!I3&amp;"',")</f>
-        <v>'Super Daddys',</v>
+        <v>'t',</v>
       </c>
       <c r="J3" t="str">
         <f>IF(ISBLANK(trends!J3),"","'"&amp;trends!J3&amp;"',")</f>
-        <v>'Downaging',</v>
+        <v>'y',</v>
       </c>
       <c r="K3" t="str">
         <f>IF(ISBLANK(trends!K3),"","'"&amp;trends!K3&amp;"',")</f>
-        <v>'24/7 Gesellschaft',</v>
+        <v>'m',</v>
       </c>
       <c r="L3" t="str">
         <f>IF(ISBLANK(trends!L3),"","'"&amp;trends!L3&amp;"',")</f>
-        <v>'Super-Safe-Society',</v>
+        <v>'s',</v>
       </c>
       <c r="M3" t="str">
         <f>IF(ISBLANK(trends!M3),"","'"&amp;trends!M3&amp;"',")</f>
@@ -1673,51 +1781,51 @@
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="str">
         <f>IF(ISBLANK(trends!A4),"","'"&amp;trends!A4&amp;"',")</f>
-        <v>'Informationsdesign',</v>
+        <v>'Open Science',</v>
       </c>
       <c r="B4" t="str">
         <f>IF(ISBLANK(trends!B4),"","'"&amp;trends!B4&amp;"',")</f>
-        <v>'E-Commerce',</v>
+        <v>'Augmented Reality',</v>
       </c>
       <c r="C4" t="str">
         <f>IF(ISBLANK(trends!C4),"","'"&amp;trends!C4&amp;"',")</f>
-        <v>'Third Places',</v>
+        <v>'Bevölkerungswachstum',</v>
       </c>
       <c r="D4" t="str">
         <f>IF(ISBLANK(trends!D4),"","'"&amp;trends!D4&amp;"',")</f>
-        <v>'Post-Carbon-Gesellschaft',</v>
+        <v>'Nachhaltigkeitsgesellschaft',</v>
       </c>
       <c r="E4" t="str">
         <f>IF(ISBLANK(trends!E4),"","'"&amp;trends!E4&amp;"',")</f>
-        <v>'Multipolare Weltordnung',</v>
+        <v>'Glokalisierung',</v>
       </c>
       <c r="F4" t="str">
         <f>IF(ISBLANK(trends!F4),"","'"&amp;trends!F4&amp;"',")</f>
-        <v>'Lebensqualität',</v>
+        <v>'Single-Gesellschaft',</v>
       </c>
       <c r="G4" t="str">
         <f>IF(ISBLANK(trends!G4),"","'"&amp;trends!G4&amp;"',")</f>
-        <v>'Detoxing',</v>
+        <v>'Sportivity',</v>
       </c>
       <c r="H4" t="str">
         <f>IF(ISBLANK(trends!H4),"","'"&amp;trends!H4&amp;"',")</f>
-        <v>'Outsourcing-Gesellschaft',</v>
+        <v>'Work-Design',</v>
       </c>
       <c r="I4" t="str">
         <f>IF(ISBLANK(trends!I4),"","'"&amp;trends!I4&amp;"',")</f>
-        <v>'Alpha Softies',</v>
+        <v>'Super Daddys',</v>
       </c>
       <c r="J4" t="str">
         <f>IF(ISBLANK(trends!J4),"","'"&amp;trends!J4&amp;"',")</f>
-        <v>'Ageless Consuming',</v>
+        <v>'Downaging',</v>
       </c>
       <c r="K4" t="str">
         <f>IF(ISBLANK(trends!K4),"","'"&amp;trends!K4&amp;"',")</f>
-        <v>'Carsharing',</v>
+        <v>'24/7 Gesellschaft',</v>
       </c>
       <c r="L4" t="str">
         <f>IF(ISBLANK(trends!L4),"","'"&amp;trends!L4&amp;"',")</f>
-        <v>'Trust Technology',</v>
+        <v>'Super-Safe-Society',</v>
       </c>
       <c r="M4" t="str">
         <f>IF(ISBLANK(trends!M4),"","'"&amp;trends!M4&amp;"',")</f>
@@ -1739,51 +1847,51 @@
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="str">
         <f>IF(ISBLANK(trends!A5),"","'"&amp;trends!A5&amp;"',")</f>
-        <v>'Bildungsbusiness',</v>
+        <v>'Informationsdesign',</v>
       </c>
       <c r="B5" t="str">
         <f>IF(ISBLANK(trends!B5),"","'"&amp;trends!B5&amp;"',")</f>
-        <v>'Crowd Funding',</v>
+        <v>'E-Commerce',</v>
       </c>
       <c r="C5" t="str">
         <f>IF(ISBLANK(trends!C5),"","'"&amp;trends!C5&amp;"',")</f>
-        <v>'Collaborative Living',</v>
+        <v>'Third Places',</v>
       </c>
       <c r="D5" t="str">
         <f>IF(ISBLANK(trends!D5),"","'"&amp;trends!D5&amp;"',")</f>
-        <v>'Bio-Boom',</v>
+        <v>'Post-Carbon-Gesellschaft',</v>
       </c>
       <c r="E5" t="str">
         <f>IF(ISBLANK(trends!E5),"","'"&amp;trends!E5&amp;"',")</f>
-        <v>'Cybercrime',</v>
+        <v>'Multipolare Weltordnung',</v>
       </c>
       <c r="F5" t="str">
         <f>IF(ISBLANK(trends!F5),"","'"&amp;trends!F5&amp;"',")</f>
-        <v>'Selftracking',</v>
+        <v>'Lebensqualität',</v>
       </c>
       <c r="G5" t="str">
         <f>IF(ISBLANK(trends!G5),"","'"&amp;trends!G5&amp;"',")</f>
-        <v>'Komplementärmedizin',</v>
+        <v>'Detoxing',</v>
       </c>
       <c r="H5" t="str">
         <f>IF(ISBLANK(trends!H5),"","'"&amp;trends!H5&amp;"',")</f>
-        <v>'Start-up-Culture',</v>
+        <v>'Outsourcing-Gesellschaft',</v>
       </c>
       <c r="I5" t="str">
         <f>IF(ISBLANK(trends!I5),"","'"&amp;trends!I5&amp;"',")</f>
-        <v>'Sexdesign',</v>
+        <v>'Alpha Softies',</v>
       </c>
       <c r="J5" t="str">
         <f>IF(ISBLANK(trends!J5),"","'"&amp;trends!J5&amp;"',")</f>
-        <v>'Forever Youngsters',</v>
+        <v>'Ageless Consuming',</v>
       </c>
       <c r="K5" t="str">
         <f>IF(ISBLANK(trends!K5),"","'"&amp;trends!K5&amp;"',")</f>
-        <v>'Autonomes Fahren',</v>
+        <v>'Carsharing',</v>
       </c>
       <c r="L5" t="str">
         <f>IF(ISBLANK(trends!L5),"","'"&amp;trends!L5&amp;"',")</f>
-        <v>'Transparenz-Märkte',</v>
+        <v>'Trust Technology',</v>
       </c>
       <c r="M5" t="str">
         <f>IF(ISBLANK(trends!M5),"","'"&amp;trends!M5&amp;"',")</f>
@@ -1805,51 +1913,51 @@
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="str">
         <f>IF(ISBLANK(trends!A6),"","'"&amp;trends!A6&amp;"',")</f>
-        <v>'Massive Open Online Course',</v>
+        <v>'Bildungsbusiness',</v>
       </c>
       <c r="B6" t="str">
         <f>IF(ISBLANK(trends!B6),"","'"&amp;trends!B6&amp;"',")</f>
-        <v>'FinTech',</v>
+        <v>'Crowd Funding',</v>
       </c>
       <c r="C6" t="str">
         <f>IF(ISBLANK(trends!C6),"","'"&amp;trends!C6&amp;"',")</f>
-        <v>'Urban Manufacturing',</v>
+        <v>'Collaborative Living',</v>
       </c>
       <c r="D6" t="str">
         <f>IF(ISBLANK(trends!D6),"","'"&amp;trends!D6&amp;"',")</f>
-        <v>'Gutbürger',</v>
+        <v>'Bio-Boom',</v>
       </c>
       <c r="E6" t="str">
         <f>IF(ISBLANK(trends!E6),"","'"&amp;trends!E6&amp;"',")</f>
-        <v>'On-demand Business',</v>
+        <v>'Cybercrime',</v>
       </c>
       <c r="F6" t="str">
         <f>IF(ISBLANK(trends!F6),"","'"&amp;trends!F6&amp;"',")</f>
-        <v>'Identitätsmanagement',</v>
+        <v>'Selftracking',</v>
       </c>
       <c r="G6" t="str">
         <f>IF(ISBLANK(trends!G6),"","'"&amp;trends!G6&amp;"',")</f>
-        <v>'Lebensqualität',</v>
+        <v>'Komplementärmedizin',</v>
       </c>
       <c r="H6" t="str">
         <f>IF(ISBLANK(trends!H6),"","'"&amp;trends!H6&amp;"',")</f>
-        <v>'Slash-Slash-Biografien',</v>
+        <v>'Start-up-Culture',</v>
       </c>
       <c r="I6" t="str">
         <f>IF(ISBLANK(trends!I6),"","'"&amp;trends!I6&amp;"',")</f>
-        <v>'Proll-Professionals',</v>
+        <v>'Sexdesign',</v>
       </c>
       <c r="J6" t="str">
         <f>IF(ISBLANK(trends!J6),"","'"&amp;trends!J6&amp;"',")</f>
-        <v>'E-Health',</v>
+        <v>'Forever Youngsters',</v>
       </c>
       <c r="K6" t="str">
         <f>IF(ISBLANK(trends!K6),"","'"&amp;trends!K6&amp;"',")</f>
-        <v>'Third Places',</v>
+        <v>'Autonomes Fahren',</v>
       </c>
       <c r="L6" t="str">
         <f>IF(ISBLANK(trends!L6),"","'"&amp;trends!L6&amp;"',")</f>
-        <v>'E-Health',</v>
+        <v>'Transparenz-Märkte',</v>
       </c>
       <c r="M6" t="str">
         <f>IF(ISBLANK(trends!M6),"","'"&amp;trends!M6&amp;"',")</f>
@@ -1871,51 +1979,51 @@
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="str">
         <f>IF(ISBLANK(trends!A7),"","'"&amp;trends!A7&amp;"',")</f>
-        <v>'Gamification',</v>
+        <v>'Massive Open Online Course',</v>
       </c>
       <c r="B7" t="str">
         <f>IF(ISBLANK(trends!B7),"","'"&amp;trends!B7&amp;"',")</f>
-        <v>'Industrie 4.0',</v>
+        <v>'FinTech',</v>
       </c>
       <c r="C7" t="str">
         <f>IF(ISBLANK(trends!C7),"","'"&amp;trends!C7&amp;"',")</f>
-        <v>'Urban Mining',</v>
+        <v>'Urban Manufacturing',</v>
       </c>
       <c r="D7" t="str">
         <f>IF(ISBLANK(trends!D7),"","'"&amp;trends!D7&amp;"',")</f>
-        <v>'Slow Culture',</v>
+        <v>'Gutbürger',</v>
       </c>
       <c r="E7" t="str">
         <f>IF(ISBLANK(trends!E7),"","'"&amp;trends!E7&amp;"',")</f>
-        <v>'Near-shoring',</v>
+        <v>'On-demand Business',</v>
       </c>
       <c r="F7" t="str">
         <f>IF(ISBLANK(trends!F7),"","'"&amp;trends!F7&amp;"',")</f>
-        <v>'Me-Cloud',</v>
+        <v>'Identitätsmanagement',</v>
       </c>
       <c r="G7" t="str">
         <f>IF(ISBLANK(trends!G7),"","'"&amp;trends!G7&amp;"',")</f>
-        <v>'Selftracking',</v>
+        <v>'Lebensqualität',</v>
       </c>
       <c r="H7" t="str">
         <f>IF(ISBLANK(trends!H7),"","'"&amp;trends!H7&amp;"',")</f>
-        <v>'Permanent Beta',</v>
+        <v>'Slash-Slash-Biografien',</v>
       </c>
       <c r="I7" t="str">
         <f>IF(ISBLANK(trends!I7),"","'"&amp;trends!I7&amp;"',")</f>
-        <v>'Work-Life-Blending',</v>
+        <v>'Proll-Professionals',</v>
       </c>
       <c r="J7" t="str">
         <f>IF(ISBLANK(trends!J7),"","'"&amp;trends!J7&amp;"',")</f>
-        <v>'Ambient Assisted Living',</v>
+        <v>'E-Health',</v>
       </c>
       <c r="K7" t="str">
         <f>IF(ISBLANK(trends!K7),"","'"&amp;trends!K7&amp;"',")</f>
-        <v>'Power of Place',</v>
+        <v>'Third Places',</v>
       </c>
       <c r="L7" t="str">
         <f>IF(ISBLANK(trends!L7),"","'"&amp;trends!L7&amp;"',")</f>
-        <v>'Identitätsmanagement',</v>
+        <v>'E-Health',</v>
       </c>
       <c r="M7" t="str">
         <f>IF(ISBLANK(trends!M7),"","'"&amp;trends!M7&amp;"',")</f>
@@ -1937,51 +2045,51 @@
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="str">
         <f>IF(ISBLANK(trends!A8),"","'"&amp;trends!A8&amp;"',")</f>
-        <v>'Predictive Analytics',</v>
+        <v>'Gamification',</v>
       </c>
       <c r="B8" t="str">
         <f>IF(ISBLANK(trends!B8),"","'"&amp;trends!B8&amp;"',")</f>
-        <v>'Big Data',</v>
+        <v>'Industrie 4.0',</v>
       </c>
       <c r="C8" t="str">
         <f>IF(ISBLANK(trends!C8),"","'"&amp;trends!C8&amp;"',")</f>
-        <v>'Urban Farming',</v>
+        <v>'Urban Mining',</v>
       </c>
       <c r="D8" t="str">
         <f>IF(ISBLANK(trends!D8),"","'"&amp;trends!D8&amp;"',")</f>
-        <v>'Maker Movement',</v>
+        <v>'Slow Culture',</v>
       </c>
       <c r="E8" t="str">
         <f>IF(ISBLANK(trends!E8),"","'"&amp;trends!E8&amp;"',")</f>
-        <v>'Schattenökonomie',</v>
+        <v>'Near-shoring',</v>
       </c>
       <c r="F8" t="str">
         <f>IF(ISBLANK(trends!F8),"","'"&amp;trends!F8&amp;"',")</f>
-        <v>'Small-World-Networks',</v>
+        <v>'Me-Cloud',</v>
       </c>
       <c r="G8" t="str">
         <f>IF(ISBLANK(trends!G8),"","'"&amp;trends!G8&amp;"',")</f>
-        <v>'E-Health',</v>
+        <v>'Selftracking',</v>
       </c>
       <c r="H8" t="str">
         <f>IF(ISBLANK(trends!H8),"","'"&amp;trends!H8&amp;"',")</f>
-        <v>'Silver Potentials',</v>
+        <v>'Permanent Beta',</v>
       </c>
       <c r="I8" t="str">
         <f>IF(ISBLANK(trends!I8),"","'"&amp;trends!I8&amp;"',")</f>
-        <v>'Diversity',</v>
+        <v>'Work-Life-Blending',</v>
       </c>
       <c r="J8" t="str">
         <f>IF(ISBLANK(trends!J8),"","'"&amp;trends!J8&amp;"',")</f>
-        <v>'Slow Culture',</v>
+        <v>'Ambient Assisted Living',</v>
       </c>
       <c r="K8" t="str">
         <f>IF(ISBLANK(trends!K8),"","'"&amp;trends!K8&amp;"',")</f>
-        <v>'Wearables',</v>
+        <v>'Power of Place',</v>
       </c>
       <c r="L8" t="str">
         <f>IF(ISBLANK(trends!L8),"","'"&amp;trends!L8&amp;"',")</f>
-        <v>'Digital Reputation',</v>
+        <v>'Identitätsmanagement',</v>
       </c>
       <c r="M8" t="str">
         <f>IF(ISBLANK(trends!M8),"","'"&amp;trends!M8&amp;"',")</f>
@@ -2003,51 +2111,51 @@
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="str">
         <f>IF(ISBLANK(trends!A9),"","'"&amp;trends!A9&amp;"',")</f>
-        <v>'Talentismus',</v>
+        <v>'Predictive Analytics',</v>
       </c>
       <c r="B9" t="str">
         <f>IF(ISBLANK(trends!B9),"","'"&amp;trends!B9&amp;"',")</f>
-        <v>'Cybercrime',</v>
+        <v>'Big Data',</v>
       </c>
       <c r="C9" t="str">
         <f>IF(ISBLANK(trends!C9),"","'"&amp;trends!C9&amp;"',")</f>
-        <v>'E-Mobility',</v>
+        <v>'Urban Farming',</v>
       </c>
       <c r="D9" t="str">
         <f>IF(ISBLANK(trends!D9),"","'"&amp;trends!D9&amp;"',")</f>
-        <v>'Sharing Economy',</v>
+        <v>'Maker Movement',</v>
       </c>
       <c r="E9" t="str">
         <f>IF(ISBLANK(trends!E9),"","'"&amp;trends!E9&amp;"',")</f>
-        <v>'Pop-up Money',</v>
+        <v>'Schattenökonomie',</v>
       </c>
       <c r="F9" t="str">
         <f>IF(ISBLANK(trends!F9),"","'"&amp;trends!F9&amp;"',")</f>
-        <v>'Maker Movement',</v>
+        <v>'Small-World-Networks',</v>
       </c>
       <c r="G9" t="str">
         <f>IF(ISBLANK(trends!G9),"","'"&amp;trends!G9&amp;"',")</f>
-        <v>'Ambient Assisted Living',</v>
+        <v>'E-Health',</v>
       </c>
       <c r="H9" t="str">
         <f>IF(ISBLANK(trends!H9),"","'"&amp;trends!H9&amp;"',")</f>
-        <v>'Corporate Health',</v>
+        <v>'Silver Potentials',</v>
       </c>
       <c r="I9" t="str">
         <f>IF(ISBLANK(trends!I9),"","'"&amp;trends!I9&amp;"',")</f>
-        <v>'Female Shift',</v>
+        <v>'Diversity',</v>
       </c>
       <c r="J9" t="str">
         <f>IF(ISBLANK(trends!J9),"","'"&amp;trends!J9&amp;"',")</f>
-        <v>'Diversity',</v>
+        <v>'Slow Culture',</v>
       </c>
       <c r="K9" t="str">
         <f>IF(ISBLANK(trends!K9),"","'"&amp;trends!K9&amp;"',")</f>
-        <v>'Langsamverkehr',</v>
+        <v>'Wearables',</v>
       </c>
       <c r="L9" t="str">
         <f>IF(ISBLANK(trends!L9),"","'"&amp;trends!L9&amp;"',")</f>
-        <v>'Predictive Analytics',</v>
+        <v>'Digital Reputation',</v>
       </c>
       <c r="M9" t="str">
         <f>IF(ISBLANK(trends!M9),"","'"&amp;trends!M9&amp;"',")</f>
@@ -2069,51 +2177,51 @@
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="str">
         <f>IF(ISBLANK(trends!A10),"","'"&amp;trends!A10&amp;"',")</f>
-        <v>'Open Innovation',</v>
+        <v>'Talentismus',</v>
       </c>
       <c r="B10" t="str">
         <f>IF(ISBLANK(trends!B10),"","'"&amp;trends!B10&amp;"',")</f>
-        <v>'Privacy',</v>
+        <v>'Cybercrime',</v>
       </c>
       <c r="C10" t="str">
         <f>IF(ISBLANK(trends!C10),"","'"&amp;trends!C10&amp;"',")</f>
-        <v>'Bike Boom',</v>
+        <v>'E-Mobility',</v>
       </c>
       <c r="D10" t="str">
         <f>IF(ISBLANK(trends!D10),"","'"&amp;trends!D10&amp;"',")</f>
-        <v>'Postwachstumsökonomie',</v>
+        <v>'Sharing Economy',</v>
       </c>
       <c r="E10" t="str">
         <f>IF(ISBLANK(trends!E10),"","'"&amp;trends!E10&amp;"',")</f>
-        <v>'Fair Trade',</v>
+        <v>'Pop-up Money',</v>
       </c>
       <c r="F10" t="str">
         <f>IF(ISBLANK(trends!F10),"","'"&amp;trends!F10&amp;"',")</f>
-        <v>'Diversity',</v>
+        <v>'Maker Movement',</v>
       </c>
       <c r="G10" t="str">
         <f>IF(ISBLANK(trends!G10),"","'"&amp;trends!G10&amp;"',")</f>
-        <v>'Slow Culture',</v>
+        <v>'Ambient Assisted Living',</v>
       </c>
       <c r="H10" t="str">
         <f>IF(ISBLANK(trends!H10),"","'"&amp;trends!H10&amp;"',")</f>
-        <v>'Work-Life Blending',</v>
+        <v>'Corporate Health',</v>
       </c>
       <c r="I10" t="str">
         <f>IF(ISBLANK(trends!I10),"","'"&amp;trends!I10&amp;"',")</f>
-        <v>'Womanomics',</v>
+        <v>'Female Shift',</v>
       </c>
       <c r="J10" t="str">
         <f>IF(ISBLANK(trends!J10),"","'"&amp;trends!J10&amp;"',")</f>
-        <v>'Liquid Youth',</v>
+        <v>'Diversity',</v>
       </c>
       <c r="K10" t="str">
         <f>IF(ISBLANK(trends!K10),"","'"&amp;trends!K10&amp;"',")</f>
-        <v>'E-Mobility',</v>
+        <v>'Langsamverkehr',</v>
       </c>
       <c r="L10" t="str">
         <f>IF(ISBLANK(trends!L10),"","'"&amp;trends!L10&amp;"',")</f>
-        <v>'Privacy',</v>
+        <v>'Predictive Analytics',</v>
       </c>
       <c r="M10" t="str">
         <f>IF(ISBLANK(trends!M10),"","'"&amp;trends!M10&amp;"',")</f>
@@ -2135,51 +2243,51 @@
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="str">
         <f>IF(ISBLANK(trends!A11),"","'"&amp;trends!A11&amp;"',")</f>
-        <v>'Kollaboration',</v>
+        <v>'Open Innovation',</v>
       </c>
       <c r="B11" t="str">
         <f>IF(ISBLANK(trends!B11),"","'"&amp;trends!B11&amp;"',")</f>
-        <v>'Predictive Analytics',</v>
+        <v>'Privacy',</v>
       </c>
       <c r="C11" t="str">
         <f>IF(ISBLANK(trends!C11),"","'"&amp;trends!C11&amp;"',")</f>
-        <v>'Megacities',</v>
+        <v>'Bike Boom',</v>
       </c>
       <c r="D11" t="str">
         <f>IF(ISBLANK(trends!D11),"","'"&amp;trends!D11&amp;"',")</f>
-        <v>'Social Business',</v>
+        <v>'Postwachstumsökonomie',</v>
       </c>
       <c r="E11" t="str">
         <f>IF(ISBLANK(trends!E11),"","'"&amp;trends!E11&amp;"',")</f>
-        <v>'Social Business',</v>
+        <v>'Fair Trade',</v>
       </c>
       <c r="F11" t="str">
         <f>IF(ISBLANK(trends!F11),"","'"&amp;trends!F11&amp;"',")</f>
-        <v>'Liquid Youth',</v>
+        <v>'Diversity',</v>
       </c>
       <c r="G11" t="str">
         <f>IF(ISBLANK(trends!G11),"","'"&amp;trends!G11&amp;"',")</f>
-        <v>'Work-Life-Blending',</v>
+        <v>'Slow Culture',</v>
       </c>
       <c r="H11" t="str">
         <f>IF(ISBLANK(trends!H11),"","'"&amp;trends!H11&amp;"',")</f>
-        <v>'Diversity',</v>
+        <v>'Work-Life Blending',</v>
       </c>
       <c r="I11" t="str">
         <f>IF(ISBLANK(trends!I11),"","'"&amp;trends!I11&amp;"',")</f>
-        <v>'Tiger Woman',</v>
+        <v>'Womanomics',</v>
       </c>
       <c r="J11" t="str">
         <f>IF(ISBLANK(trends!J11),"","'"&amp;trends!J11&amp;"',")</f>
-        <v>'Silver Potentials',</v>
+        <v>'Liquid Youth',</v>
       </c>
       <c r="K11" t="str">
         <f>IF(ISBLANK(trends!K11),"","'"&amp;trends!K11&amp;"',")</f>
-        <v>'Bike-Boom',</v>
+        <v>'E-Mobility',</v>
       </c>
       <c r="L11" t="str">
         <f>IF(ISBLANK(trends!L11),"","'"&amp;trends!L11&amp;"',")</f>
-        <v>'Cybercrime',</v>
+        <v>'Privacy',</v>
       </c>
       <c r="M11" t="str">
         <f>IF(ISBLANK(trends!M11),"","'"&amp;trends!M11&amp;"',")</f>
@@ -2201,51 +2309,51 @@
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="str">
         <f>IF(ISBLANK(trends!A12),"","'"&amp;trends!A12&amp;"',")</f>
-        <v>'Sharing Economy',</v>
+        <v>'Kollaboration',</v>
       </c>
       <c r="B12" t="str">
         <f>IF(ISBLANK(trends!B12),"","'"&amp;trends!B12&amp;"',")</f>
-        <v>'Selftracking',</v>
+        <v>'Predictive Analytics',</v>
       </c>
       <c r="C12" t="str">
         <f>IF(ISBLANK(trends!C12),"","'"&amp;trends!C12&amp;"',")</f>
-        <v>'Global Cities',</v>
+        <v>'Megacities',</v>
       </c>
       <c r="D12" t="str">
         <f>IF(ISBLANK(trends!D12),"","'"&amp;trends!D12&amp;"',")</f>
-        <v>'Fair Trade',</v>
+        <v>'Social Business',</v>
       </c>
       <c r="E12" t="str">
         <f>IF(ISBLANK(trends!E12),"","'"&amp;trends!E12&amp;"',")</f>
-        <v>'Postwachstumsökonomie',</v>
+        <v>'Social Business',</v>
       </c>
       <c r="F12" t="str">
         <f>IF(ISBLANK(trends!F12),"","'"&amp;trends!F12&amp;"',")</f>
-        <v>'Multigrafie',</v>
+        <v>'Liquid Youth',</v>
       </c>
       <c r="G12" t="str">
         <f>IF(ISBLANK(trends!G12),"","'"&amp;trends!G12&amp;"',")</f>
-        <v>'Corporate Health',</v>
+        <v>'Work-Life-Blending',</v>
       </c>
       <c r="H12" t="str">
         <f>IF(ISBLANK(trends!H12),"","'"&amp;trends!H12&amp;"',")</f>
-        <v>'Female Shift',</v>
+        <v>'Diversity',</v>
       </c>
       <c r="I12" t="str">
         <f>IF(ISBLANK(trends!I12),"","'"&amp;trends!I12&amp;"',")</f>
-        <v>'Regenbogenfamilien',</v>
+        <v>'Tiger Woman',</v>
       </c>
       <c r="J12" t="str">
         <f>IF(ISBLANK(trends!J12),"","'"&amp;trends!J12&amp;"',")</f>
-        <v>'Healthness',</v>
+        <v>'Silver Potentials',</v>
       </c>
       <c r="K12" t="str">
         <f>IF(ISBLANK(trends!K12),"","'"&amp;trends!K12&amp;"',")</f>
-        <v>'Unterwegsmärkte',</v>
+        <v>'Bike-Boom',</v>
       </c>
       <c r="L12" t="str">
         <f>IF(ISBLANK(trends!L12),"","'"&amp;trends!L12&amp;"',")</f>
-        <v>'Big Data',</v>
+        <v>'Cybercrime',</v>
       </c>
       <c r="M12" t="str">
         <f>IF(ISBLANK(trends!M12),"","'"&amp;trends!M12&amp;"',")</f>
@@ -2267,51 +2375,51 @@
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" t="str">
         <f>IF(ISBLANK(trends!A13),"","'"&amp;trends!A13&amp;"',")</f>
-        <v>'Female Shift',</v>
+        <v>'Sharing Economy',</v>
       </c>
       <c r="B13" t="str">
         <f>IF(ISBLANK(trends!B13),"","'"&amp;trends!B13&amp;"',")</f>
-        <v>'E-Health',</v>
+        <v>'Selftracking',</v>
       </c>
       <c r="C13" t="str">
         <f>IF(ISBLANK(trends!C13),"","'"&amp;trends!C13&amp;"',")</f>
-        <v>'Landflucht',</v>
+        <v>'Global Cities',</v>
       </c>
       <c r="D13" t="str">
         <f>IF(ISBLANK(trends!D13),"","'"&amp;trends!D13&amp;"',")</f>
-        <v>'Swapping',</v>
+        <v>'Fair Trade',</v>
       </c>
       <c r="E13" t="str">
         <f>IF(ISBLANK(trends!E13),"","'"&amp;trends!E13&amp;"',")</f>
-        <v>'Womanomics',</v>
+        <v>'Postwachstumsökonomie',</v>
       </c>
       <c r="F13" t="str">
         <f>IF(ISBLANK(trends!F13),"","'"&amp;trends!F13&amp;"',")</f>
-        <v>'Tutorial Learning',</v>
+        <v>'Multigrafie',</v>
       </c>
       <c r="G13" t="str">
         <f>IF(ISBLANK(trends!G13),"","'"&amp;trends!G13&amp;"',")</f>
-        <v>'Healthness',</v>
+        <v>'Corporate Health',</v>
       </c>
       <c r="H13" t="str">
         <f>IF(ISBLANK(trends!H13),"","'"&amp;trends!H13&amp;"',")</f>
-        <v>'Womanomics',</v>
+        <v>'Female Shift',</v>
       </c>
       <c r="I13" t="str">
         <f>IF(ISBLANK(trends!I13),"","'"&amp;trends!I13&amp;"',")</f>
-        <v>'Neue Mütter',</v>
+        <v>'Regenbogenfamilien',</v>
       </c>
       <c r="J13" t="str">
         <f>IF(ISBLANK(trends!J13),"","'"&amp;trends!J13&amp;"',")</f>
-        <v>'Universal Design',</v>
+        <v>'Healthness',</v>
       </c>
       <c r="K13" t="str">
         <f>IF(ISBLANK(trends!K13),"","'"&amp;trends!K13&amp;"',")</f>
-        <v>'Mobile Commerce',</v>
+        <v>'Unterwegsmärkte',</v>
       </c>
       <c r="L13" t="str">
         <f>IF(ISBLANK(trends!L13),"","'"&amp;trends!L13&amp;"',")</f>
-        <v>'Industrie 4.0',</v>
+        <v>'Big Data',</v>
       </c>
       <c r="M13" t="str">
         <f>IF(ISBLANK(trends!M13),"","'"&amp;trends!M13&amp;"',")</f>
@@ -2333,51 +2441,51 @@
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" t="str">
         <f>IF(ISBLANK(trends!A14),"","'"&amp;trends!A14&amp;"',")</f>
-        <v>'Life-Long-Learning',</v>
+        <v>'Female Shift',</v>
       </c>
       <c r="B14" t="str">
         <f>IF(ISBLANK(trends!B14),"","'"&amp;trends!B14&amp;"',")</f>
-        <v>'Me-Cloud',</v>
+        <v>'E-Health',</v>
       </c>
       <c r="C14" t="str">
         <f>IF(ISBLANK(trends!C14),"","'"&amp;trends!C14&amp;"',")</f>
-        <v>'Schrumpfende Städte',</v>
+        <v>'Landflucht',</v>
       </c>
       <c r="D14" t="str">
         <f>IF(ISBLANK(trends!D14),"","'"&amp;trends!D14&amp;"',")</f>
-        <v>'Zero Waste',</v>
+        <v>'Swapping',</v>
       </c>
       <c r="E14" t="str">
         <f>IF(ISBLANK(trends!E14),"","'"&amp;trends!E14&amp;"',")</f>
-        <v>'Rising Africa',</v>
+        <v>'Womanomics',</v>
       </c>
       <c r="F14" t="str">
         <f>IF(ISBLANK(trends!F14),"","'"&amp;trends!F14&amp;"',")</f>
-        <v>'Regenbogenfamilien',</v>
+        <v>'Tutorial Learning',</v>
       </c>
       <c r="G14" t="str">
         <f>IF(ISBLANK(trends!G14),"","'"&amp;trends!G14&amp;"',")</f>
-        <v>'Foodies',</v>
+        <v>'Healthness',</v>
       </c>
       <c r="H14" t="str">
         <f>IF(ISBLANK(trends!H14),"","'"&amp;trends!H14&amp;"',")</f>
-        <v>'Co-Working',</v>
+        <v>'Womanomics',</v>
       </c>
       <c r="I14" t="str">
         <f>IF(ISBLANK(trends!I14),"","'"&amp;trends!I14&amp;"',")</f>
-        <v>'Phasenfamilien',</v>
+        <v>'Neue Mütter',</v>
       </c>
       <c r="J14" t="str">
         <f>IF(ISBLANK(trends!J14),"","'"&amp;trends!J14&amp;"',")</f>
-        <v/>
+        <v>'Universal Design',</v>
       </c>
       <c r="K14" t="str">
         <f>IF(ISBLANK(trends!K14),"","'"&amp;trends!K14&amp;"',")</f>
-        <v>'Mixed Mobility',</v>
+        <v>'Mobile Commerce',</v>
       </c>
       <c r="L14" t="str">
         <f>IF(ISBLANK(trends!L14),"","'"&amp;trends!L14&amp;"',")</f>
-        <v>'Flexicurity',</v>
+        <v>'Industrie 4.0',</v>
       </c>
       <c r="M14" t="str">
         <f>IF(ISBLANK(trends!M14),"","'"&amp;trends!M14&amp;"',")</f>
@@ -2399,39 +2507,39 @@
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" t="str">
         <f>IF(ISBLANK(trends!A15),"","'"&amp;trends!A15&amp;"',")</f>
-        <v>'Tutorial Learning',</v>
+        <v>'Life-Long-Learning',</v>
       </c>
       <c r="B15" t="str">
         <f>IF(ISBLANK(trends!B15),"","'"&amp;trends!B15&amp;"',")</f>
-        <v>'Open Innovation',</v>
+        <v>'Me-Cloud',</v>
       </c>
       <c r="C15" t="str">
         <f>IF(ISBLANK(trends!C15),"","'"&amp;trends!C15&amp;"',")</f>
-        <v>'Smart Cities',</v>
+        <v>'Schrumpfende Städte',</v>
       </c>
       <c r="D15" t="str">
         <f>IF(ISBLANK(trends!D15),"","'"&amp;trends!D15&amp;"',")</f>
-        <v>'Green Tech',</v>
+        <v>'Zero Waste',</v>
       </c>
       <c r="E15" t="str">
         <f>IF(ISBLANK(trends!E15),"","'"&amp;trends!E15&amp;"',")</f>
-        <v>'Weltmacht China',</v>
+        <v>'Rising Africa',</v>
       </c>
       <c r="F15" t="str">
         <f>IF(ISBLANK(trends!F15),"","'"&amp;trends!F15&amp;"',")</f>
-        <v>'Wir-Kultur',</v>
+        <v>'Regenbogenfamilien',</v>
       </c>
       <c r="G15" t="str">
         <f>IF(ISBLANK(trends!G15),"","'"&amp;trends!G15&amp;"',")</f>
-        <v>'Lebensenergie',</v>
+        <v>'Foodies',</v>
       </c>
       <c r="H15" t="str">
         <f>IF(ISBLANK(trends!H15),"","'"&amp;trends!H15&amp;"',")</f>
-        <v>'Service-Ökonomie',</v>
+        <v>'Co-Working',</v>
       </c>
       <c r="I15" t="str">
         <f>IF(ISBLANK(trends!I15),"","'"&amp;trends!I15&amp;"',")</f>
-        <v/>
+        <v>'Phasenfamilien',</v>
       </c>
       <c r="J15" t="str">
         <f>IF(ISBLANK(trends!J15),"","'"&amp;trends!J15&amp;"',")</f>
@@ -2439,11 +2547,11 @@
       </c>
       <c r="K15" t="str">
         <f>IF(ISBLANK(trends!K15),"","'"&amp;trends!K15&amp;"',")</f>
-        <v>'End-to-End-Tourismus',</v>
+        <v>'Mixed Mobility',</v>
       </c>
       <c r="L15" t="str">
         <f>IF(ISBLANK(trends!L15),"","'"&amp;trends!L15&amp;"',")</f>
-        <v>'Antifragilität',</v>
+        <v>'Flexicurity',</v>
       </c>
       <c r="M15" t="str">
         <f>IF(ISBLANK(trends!M15),"","'"&amp;trends!M15&amp;"',")</f>
@@ -2465,35 +2573,35 @@
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" t="str">
         <f>IF(ISBLANK(trends!A16),"","'"&amp;trends!A16&amp;"',")</f>
-        <v>'Creativiteens',</v>
+        <v>'Tutorial Learning',</v>
       </c>
       <c r="B16" t="str">
         <f>IF(ISBLANK(trends!B16),"","'"&amp;trends!B16&amp;"',")</f>
-        <v>'Pop-up Money',</v>
+        <v>'Open Innovation',</v>
       </c>
       <c r="C16" t="str">
         <f>IF(ISBLANK(trends!C16),"","'"&amp;trends!C16&amp;"',")</f>
-        <v/>
+        <v>'Smart Cities',</v>
       </c>
       <c r="D16" t="str">
         <f>IF(ISBLANK(trends!D16),"","'"&amp;trends!D16&amp;"',")</f>
-        <v>'Urban Farming',</v>
+        <v>'Green Tech',</v>
       </c>
       <c r="E16" t="str">
         <f>IF(ISBLANK(trends!E16),"","'"&amp;trends!E16&amp;"',")</f>
-        <v>'Global Cities',</v>
+        <v>'Weltmacht China',</v>
       </c>
       <c r="F16" t="str">
         <f>IF(ISBLANK(trends!F16),"","'"&amp;trends!F16&amp;"',")</f>
-        <v/>
+        <v>'Wir-Kultur',</v>
       </c>
       <c r="G16" t="str">
         <f>IF(ISBLANK(trends!G16),"","'"&amp;trends!G16&amp;"',")</f>
-        <v>'Achtsamkeit',</v>
+        <v>'Lebensenergie',</v>
       </c>
       <c r="H16" t="str">
         <f>IF(ISBLANK(trends!H16),"","'"&amp;trends!H16&amp;"',")</f>
-        <v>'Social Business',</v>
+        <v>'Service-Ökonomie',</v>
       </c>
       <c r="I16" t="str">
         <f>IF(ISBLANK(trends!I16),"","'"&amp;trends!I16&amp;"',")</f>
@@ -2505,11 +2613,11 @@
       </c>
       <c r="K16" t="str">
         <f>IF(ISBLANK(trends!K16),"","'"&amp;trends!K16&amp;"',")</f>
-        <v/>
+        <v>'End-to-End-Tourismus',</v>
       </c>
       <c r="L16" t="str">
         <f>IF(ISBLANK(trends!L16),"","'"&amp;trends!L16&amp;"',")</f>
-        <v>'Simplexity',</v>
+        <v>'Antifragilität',</v>
       </c>
       <c r="M16" t="str">
         <f>IF(ISBLANK(trends!M16),"","'"&amp;trends!M16&amp;"',")</f>
@@ -2531,11 +2639,11 @@
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" t="str">
         <f>IF(ISBLANK(trends!A17),"","'"&amp;trends!A17&amp;"',")</f>
-        <v>'Neugiermanagement',</v>
+        <v>'Creativiteens',</v>
       </c>
       <c r="B17" t="str">
         <f>IF(ISBLANK(trends!B17),"","'"&amp;trends!B17&amp;"',")</f>
-        <v>'Swapping',</v>
+        <v>'Pop-up Money',</v>
       </c>
       <c r="C17" t="str">
         <f>IF(ISBLANK(trends!C17),"","'"&amp;trends!C17&amp;"',")</f>
@@ -2543,11 +2651,11 @@
       </c>
       <c r="D17" t="str">
         <f>IF(ISBLANK(trends!D17),"","'"&amp;trends!D17&amp;"',")</f>
-        <v>'E-Mobility',</v>
+        <v>'Urban Farming',</v>
       </c>
       <c r="E17" t="str">
         <f>IF(ISBLANK(trends!E17),"","'"&amp;trends!E17&amp;"',")</f>
-        <v>'Migration',</v>
+        <v>'Global Cities',</v>
       </c>
       <c r="F17" t="str">
         <f>IF(ISBLANK(trends!F17),"","'"&amp;trends!F17&amp;"',")</f>
@@ -2555,11 +2663,11 @@
       </c>
       <c r="G17" t="str">
         <f>IF(ISBLANK(trends!G17),"","'"&amp;trends!G17&amp;"',")</f>
-        <v/>
+        <v>'Achtsamkeit',</v>
       </c>
       <c r="H17" t="str">
         <f>IF(ISBLANK(trends!H17),"","'"&amp;trends!H17&amp;"',")</f>
-        <v>'Kollaboration',</v>
+        <v>'Social Business',</v>
       </c>
       <c r="I17" t="str">
         <f>IF(ISBLANK(trends!I17),"","'"&amp;trends!I17&amp;"',")</f>
@@ -2575,7 +2683,7 @@
       </c>
       <c r="L17" t="str">
         <f>IF(ISBLANK(trends!L17),"","'"&amp;trends!L17&amp;"',")</f>
-        <v/>
+        <v>'Simplexity',</v>
       </c>
       <c r="M17" t="str">
         <f>IF(ISBLANK(trends!M17),"","'"&amp;trends!M17&amp;"',")</f>
@@ -2597,11 +2705,11 @@
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" t="str">
         <f>IF(ISBLANK(trends!A18),"","'"&amp;trends!A18&amp;"',")</f>
-        <v/>
+        <v>'Neugiermanagement',</v>
       </c>
       <c r="B18" t="str">
         <f>IF(ISBLANK(trends!B18),"","'"&amp;trends!B18&amp;"',")</f>
-        <v>'Smart Devices',</v>
+        <v>'Swapping',</v>
       </c>
       <c r="C18" t="str">
         <f>IF(ISBLANK(trends!C18),"","'"&amp;trends!C18&amp;"',")</f>
@@ -2609,11 +2717,11 @@
       </c>
       <c r="D18" t="str">
         <f>IF(ISBLANK(trends!D18),"","'"&amp;trends!D18&amp;"',")</f>
-        <v>'Circular Economy',</v>
+        <v>'E-Mobility',</v>
       </c>
       <c r="E18" t="str">
         <f>IF(ISBLANK(trends!E18),"","'"&amp;trends!E18&amp;"',")</f>
-        <v/>
+        <v>'Migration',</v>
       </c>
       <c r="F18" t="str">
         <f>IF(ISBLANK(trends!F18),"","'"&amp;trends!F18&amp;"',")</f>
@@ -2625,7 +2733,7 @@
       </c>
       <c r="H18" t="str">
         <f>IF(ISBLANK(trends!H18),"","'"&amp;trends!H18&amp;"',")</f>
-        <v>'Open Innovation',</v>
+        <v>'Kollaboration',</v>
       </c>
       <c r="I18" t="str">
         <f>IF(ISBLANK(trends!I18),"","'"&amp;trends!I18&amp;"',")</f>
@@ -2667,7 +2775,7 @@
       </c>
       <c r="B19" t="str">
         <f>IF(ISBLANK(trends!B19),"","'"&amp;trends!B19&amp;"',")</f>
-        <v>'Internet der Dinge',</v>
+        <v>'Smart Devices',</v>
       </c>
       <c r="C19" t="str">
         <f>IF(ISBLANK(trends!C19),"","'"&amp;trends!C19&amp;"',")</f>
@@ -2675,7 +2783,7 @@
       </c>
       <c r="D19" t="str">
         <f>IF(ISBLANK(trends!D19),"","'"&amp;trends!D19&amp;"',")</f>
-        <v/>
+        <v>'Circular Economy',</v>
       </c>
       <c r="E19" t="str">
         <f>IF(ISBLANK(trends!E19),"","'"&amp;trends!E19&amp;"',")</f>
@@ -2691,7 +2799,7 @@
       </c>
       <c r="H19" t="str">
         <f>IF(ISBLANK(trends!H19),"","'"&amp;trends!H19&amp;"',")</f>
-        <v>'Talentismus',</v>
+        <v>'Open Innovation',</v>
       </c>
       <c r="I19" t="str">
         <f>IF(ISBLANK(trends!I19),"","'"&amp;trends!I19&amp;"',")</f>
@@ -2733,7 +2841,7 @@
       </c>
       <c r="B20" t="str">
         <f>IF(ISBLANK(trends!B20),"","'"&amp;trends!B20&amp;"',")</f>
-        <v>'Social Networks',</v>
+        <v>'Internet der Dinge',</v>
       </c>
       <c r="C20" t="str">
         <f>IF(ISBLANK(trends!C20),"","'"&amp;trends!C20&amp;"',")</f>
@@ -2757,7 +2865,7 @@
       </c>
       <c r="H20" t="str">
         <f>IF(ISBLANK(trends!H20),"","'"&amp;trends!H20&amp;"',")</f>
-        <v>'On-demand Business',</v>
+        <v>'Talentismus',</v>
       </c>
       <c r="I20" t="str">
         <f>IF(ISBLANK(trends!I20),"","'"&amp;trends!I20&amp;"',")</f>
@@ -2799,7 +2907,7 @@
       </c>
       <c r="B21" t="str">
         <f>IF(ISBLANK(trends!B21),"","'"&amp;trends!B21&amp;"',")</f>
-        <v/>
+        <v>'Social Networks',</v>
       </c>
       <c r="C21" t="str">
         <f>IF(ISBLANK(trends!C21),"","'"&amp;trends!C21&amp;"',")</f>
@@ -2823,7 +2931,7 @@
       </c>
       <c r="H21" t="str">
         <f>IF(ISBLANK(trends!H21),"","'"&amp;trends!H21&amp;"',")</f>
-        <v>'Flexicurity',</v>
+        <v>'On-demand Business',</v>
       </c>
       <c r="I21" t="str">
         <f>IF(ISBLANK(trends!I21),"","'"&amp;trends!I21&amp;"',")</f>
@@ -2889,7 +2997,7 @@
       </c>
       <c r="H22" t="str">
         <f>IF(ISBLANK(trends!H22),"","'"&amp;trends!H22&amp;"',")</f>
-        <v>'Antifragilität',</v>
+        <v>'Flexicurity',</v>
       </c>
       <c r="I22" t="str">
         <f>IF(ISBLANK(trends!I22),"","'"&amp;trends!I22&amp;"',")</f>
@@ -2955,7 +3063,7 @@
       </c>
       <c r="H23" t="str">
         <f>IF(ISBLANK(trends!H23),"","'"&amp;trends!H23&amp;"',")</f>
-        <v>'Urban Manufacturing',</v>
+        <v>'Antifragilität',</v>
       </c>
       <c r="I23" t="str">
         <f>IF(ISBLANK(trends!I23),"","'"&amp;trends!I23&amp;"',")</f>
@@ -3021,7 +3129,7 @@
       </c>
       <c r="H24" t="str">
         <f>IF(ISBLANK(trends!H24),"","'"&amp;trends!H24&amp;"',")</f>
-        <v>'Power of Place',</v>
+        <v>'Urban Manufacturing',</v>
       </c>
       <c r="I24" t="str">
         <f>IF(ISBLANK(trends!I24),"","'"&amp;trends!I24&amp;"',")</f>
@@ -3087,7 +3195,7 @@
       </c>
       <c r="H25" t="str">
         <f>IF(ISBLANK(trends!H25),"","'"&amp;trends!H25&amp;"',")</f>
-        <v>'Kreativökonomie',</v>
+        <v>'Power of Place',</v>
       </c>
       <c r="I25" t="str">
         <f>IF(ISBLANK(trends!I25),"","'"&amp;trends!I25&amp;"',")</f>
@@ -3153,7 +3261,7 @@
       </c>
       <c r="H26" t="str">
         <f>IF(ISBLANK(trends!H26),"","'"&amp;trends!H26&amp;"',")</f>
-        <v/>
+        <v>'Kreativökonomie',</v>
       </c>
       <c r="I26" t="str">
         <f>IF(ISBLANK(trends!I26),"","'"&amp;trends!I26&amp;"',")</f>
@@ -3389,57 +3497,57 @@
     <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" t="str">
         <f>"["&amp;A1&amp;A2&amp;A3&amp;A4&amp;A5&amp;A6&amp;A7&amp;A8&amp;A9&amp;A10&amp;A11&amp;A12&amp;A13&amp;A14&amp;A15&amp;A16&amp;A17&amp;A18&amp;A19&amp;A20&amp;A21&amp;A22&amp;A23&amp;A24&amp;A25&amp;A26&amp;A27&amp;A28&amp;A29&amp;"],"</f>
-        <v>['Wissenskultur','konn.png','Open Science','Informationsdesign','Bildungsbusiness','Massive Open Online Course','Gamification','Predictive Analytics','Talentismus','Open Innovation','Kollaboration','Sharing Economy','Female Shift','Life-Long-Learning','Tutorial Learning','Creativiteens','Neugiermanagement',],</v>
+        <v>['Wissenskultur','Wissenskultur.svg','w','Open Science','Informationsdesign','Bildungsbusiness','Massive Open Online Course','Gamification','Predictive Analytics','Talentismus','Open Innovation','Kollaboration','Sharing Economy','Female Shift','Life-Long-Learning','Tutorial Learning','Creativiteens','Neugiermanagement',],</v>
       </c>
       <c r="B30" t="str">
-        <f t="shared" ref="B30:L30" si="0">"["&amp;B1&amp;B2&amp;B3&amp;B4&amp;B5&amp;B6&amp;B7&amp;B8&amp;B9&amp;B10&amp;B11&amp;B12&amp;B13&amp;B14&amp;B15&amp;B16&amp;B17&amp;B18&amp;B19&amp;B20&amp;B21&amp;B22&amp;B23&amp;B24&amp;B25&amp;B26&amp;B27&amp;B28&amp;B29&amp;"],"</f>
-        <v>['Konnektivität','konn.png','Augmented Reality','E-Commerce','Crowd Funding','FinTech','Industrie 4.0','Big Data','Cybercrime','Privacy','Predictive Analytics','Selftracking','E-Health','Me-Cloud','Open Innovation','Pop-up Money','Swapping','Smart Devices','Internet der Dinge','Social Networks',],</v>
+        <f>"["&amp;B1&amp;B2&amp;B3&amp;B4&amp;B5&amp;B6&amp;B7&amp;B8&amp;B9&amp;B10&amp;B11&amp;B12&amp;B13&amp;B14&amp;B15&amp;B16&amp;B17&amp;B18&amp;B19&amp;B20&amp;B21&amp;B22&amp;B23&amp;B24&amp;B25&amp;B26&amp;B27&amp;B28&amp;B29&amp;"],"</f>
+        <v>['Konnektivität','Konnektivität.svg','k','Augmented Reality','E-Commerce','Crowd Funding','FinTech','Industrie 4.0','Big Data','Cybercrime','Privacy','Predictive Analytics','Selftracking','E-Health','Me-Cloud','Open Innovation','Pop-up Money','Swapping','Smart Devices','Internet der Dinge','Social Networks',],</v>
       </c>
       <c r="C30" t="str">
-        <f t="shared" si="0"/>
-        <v>['Urbanisierung','konn.png','Bevölkerungswachstum','Third Places','Collaborative Living','Urban Manufacturing','Urban Mining','Urban Farming','E-Mobility','Bike Boom','Megacities','Global Cities','Landflucht','Schrumpfende Städte','Smart Cities',],</v>
+        <f>"["&amp;C1&amp;C2&amp;C3&amp;C4&amp;C5&amp;C6&amp;C7&amp;C8&amp;C9&amp;C10&amp;C11&amp;C12&amp;C13&amp;C14&amp;C15&amp;C16&amp;C17&amp;C18&amp;C19&amp;C20&amp;C21&amp;C22&amp;C23&amp;C24&amp;C25&amp;C26&amp;C27&amp;C28&amp;C29&amp;"],"</f>
+        <v>['Urbanisierung','Urbanisierung.svg','u','Bevölkerungswachstum','Third Places','Collaborative Living','Urban Manufacturing','Urban Mining','Urban Farming','E-Mobility','Bike Boom','Megacities','Global Cities','Landflucht','Schrumpfende Städte','Smart Cities',],</v>
       </c>
       <c r="D30" t="str">
-        <f t="shared" si="0"/>
-        <v>['Neo-Ökologie','konn.png','Nachhaltigkeitsgesellschaft','Post-Carbon-Gesellschaft','Bio-Boom','Gutbürger','Slow Culture','Maker Movement','Sharing Economy','Postwachstumsökonomie','Social Business','Fair Trade','Swapping','Zero Waste','Green Tech','Urban Farming','E-Mobility','Circular Economy',],</v>
+        <f>"["&amp;D1&amp;D2&amp;D3&amp;D4&amp;D5&amp;D6&amp;D7&amp;D8&amp;D9&amp;D10&amp;D11&amp;D12&amp;D13&amp;D14&amp;D15&amp;D16&amp;D17&amp;D18&amp;D19&amp;D20&amp;D21&amp;D22&amp;D23&amp;D24&amp;D25&amp;D26&amp;D27&amp;D28&amp;D29&amp;"],"</f>
+        <v>['Neo-Ökologie','Neo-Ökologie.svg','ö','Nachhaltigkeitsgesellschaft','Post-Carbon-Gesellschaft','Bio-Boom','Gutbürger','Slow Culture','Maker Movement','Sharing Economy','Postwachstumsökonomie','Social Business','Fair Trade','Swapping','Zero Waste','Green Tech','Urban Farming','E-Mobility','Circular Economy',],</v>
       </c>
       <c r="E30" t="str">
-        <f t="shared" si="0"/>
-        <v>['Globalisierung','konn.png','Glokalisierung','Multipolare Weltordnung','Cybercrime','On-demand Business','Near-shoring','Schattenökonomie','Pop-up Money','Fair Trade','Social Business','Postwachstumsökonomie','Womanomics','Rising Africa','Weltmacht China','Global Cities','Migration',],</v>
+        <f>"["&amp;E1&amp;E2&amp;E3&amp;E4&amp;E5&amp;E6&amp;E7&amp;E8&amp;E9&amp;E10&amp;E11&amp;E12&amp;E13&amp;E14&amp;E15&amp;E16&amp;E17&amp;E18&amp;E19&amp;E20&amp;E21&amp;E22&amp;E23&amp;E24&amp;E25&amp;E26&amp;E27&amp;E28&amp;E29&amp;"],"</f>
+        <v>['Globalisierung','Globalisierung.svg','q','Glokalisierung','Multipolare Weltordnung','Cybercrime','On-demand Business','Near-shoring','Schattenökonomie','Pop-up Money','Fair Trade','Social Business','Postwachstumsökonomie','Womanomics','Rising Africa','Weltmacht China','Global Cities','Migration',],</v>
       </c>
       <c r="F30" t="str">
-        <f t="shared" si="0"/>
-        <v>['Individualisierung','konn.png','Single-Gesellschaft','Lebensqualität','Selftracking','Identitätsmanagement','Me-Cloud','Small-World-Networks','Maker Movement','Diversity','Liquid Youth','Multigrafie','Tutorial Learning','Regenbogenfamilien','Wir-Kultur',],</v>
+        <f>"["&amp;F1&amp;F2&amp;F3&amp;F4&amp;F5&amp;F6&amp;F7&amp;F8&amp;F9&amp;F10&amp;F11&amp;F12&amp;F13&amp;F14&amp;F15&amp;F16&amp;F17&amp;F18&amp;F19&amp;F20&amp;F21&amp;F22&amp;F23&amp;F24&amp;F25&amp;F26&amp;F27&amp;F28&amp;F29&amp;"],"</f>
+        <v>['Individualisierung','Individualisierung.svg','i','Single-Gesellschaft','Lebensqualität','Selftracking','Identitätsmanagement','Me-Cloud','Small-World-Networks','Maker Movement','Diversity','Liquid Youth','Multigrafie','Tutorial Learning','Regenbogenfamilien','Wir-Kultur',],</v>
       </c>
       <c r="G30" t="str">
-        <f t="shared" si="0"/>
-        <v>['Gesundheit','konn.png','Sportivity','Detoxing','Komplementärmedizin','Lebensqualität','Selftracking','E-Health','Ambient Assisted Living','Slow Culture','Work-Life-Blending','Corporate Health','Healthness','Foodies','Lebensenergie','Achtsamkeit',],</v>
+        <f>"["&amp;G1&amp;G2&amp;G3&amp;G4&amp;G5&amp;G6&amp;G7&amp;G8&amp;G9&amp;G10&amp;G11&amp;G12&amp;G13&amp;G14&amp;G15&amp;G16&amp;G17&amp;G18&amp;G19&amp;G20&amp;G21&amp;G22&amp;G23&amp;G24&amp;G25&amp;G26&amp;G27&amp;G28&amp;G29&amp;"],"</f>
+        <v>['Gesundheit','Gesundheit.svg','g','Sportivity','Detoxing','Komplementärmedizin','Lebensqualität','Selftracking','E-Health','Ambient Assisted Living','Slow Culture','Work-Life-Blending','Corporate Health','Healthness','Foodies','Lebensenergie','Achtsamkeit',],</v>
       </c>
       <c r="H30" t="str">
-        <f t="shared" si="0"/>
-        <v>['New Work','konn.png','Work-Design','Outsourcing-Gesellschaft','Start-up-Culture','Slash-Slash-Biografien','Permanent Beta','Silver Potentials','Corporate Health','Work-Life Blending','Diversity','Female Shift','Womanomics','Co-Working','Service-Ökonomie','Social Business','Kollaboration','Open Innovation','Talentismus','On-demand Business','Flexicurity','Antifragilität','Urban Manufacturing','Power of Place','Kreativökonomie',],</v>
+        <f>"["&amp;H1&amp;H2&amp;H3&amp;H4&amp;H5&amp;H6&amp;H7&amp;H8&amp;H9&amp;H10&amp;H11&amp;H12&amp;H13&amp;H14&amp;H15&amp;H16&amp;H17&amp;H18&amp;H19&amp;H20&amp;H21&amp;H22&amp;H23&amp;H24&amp;H25&amp;H26&amp;H27&amp;H28&amp;H29&amp;"],"</f>
+        <v>['New Work','New Work.svg','n','Work-Design','Outsourcing-Gesellschaft','Start-up-Culture','Slash-Slash-Biografien','Permanent Beta','Silver Potentials','Corporate Health','Work-Life Blending','Diversity','Female Shift','Womanomics','Co-Working','Service-Ökonomie','Social Business','Kollaboration','Open Innovation','Talentismus','On-demand Business','Flexicurity','Antifragilität','Urban Manufacturing','Power of Place','Kreativökonomie',],</v>
       </c>
       <c r="I30" t="str">
-        <f t="shared" si="0"/>
-        <v>['Gender Shift','konn.png','Super Daddys','Alpha Softies','Sexdesign','Proll-Professionals','Work-Life-Blending','Diversity','Female Shift','Womanomics','Tiger Woman','Regenbogenfamilien','Neue Mütter','Phasenfamilien',],</v>
+        <f>"["&amp;I1&amp;I2&amp;I3&amp;I4&amp;I5&amp;I6&amp;I7&amp;I8&amp;I9&amp;I10&amp;I11&amp;I12&amp;I13&amp;I14&amp;I15&amp;I16&amp;I17&amp;I18&amp;I19&amp;I20&amp;I21&amp;I22&amp;I23&amp;I24&amp;I25&amp;I26&amp;I27&amp;I28&amp;I29&amp;"],"</f>
+        <v>['Gender Shift','Gender Shift.svg','t','Super Daddys','Alpha Softies','Sexdesign','Proll-Professionals','Work-Life-Blending','Diversity','Female Shift','Womanomics','Tiger Woman','Regenbogenfamilien','Neue Mütter','Phasenfamilien',],</v>
       </c>
       <c r="J30" t="str">
-        <f t="shared" si="0"/>
-        <v>['Silver Society','konn.png','Downaging','Ageless Consuming','Forever Youngsters','E-Health','Ambient Assisted Living','Slow Culture','Diversity','Liquid Youth','Silver Potentials','Healthness','Universal Design',],</v>
+        <f>"["&amp;J1&amp;J2&amp;J3&amp;J4&amp;J5&amp;J6&amp;J7&amp;J8&amp;J9&amp;J10&amp;J11&amp;J12&amp;J13&amp;J14&amp;J15&amp;J16&amp;J17&amp;J18&amp;J19&amp;J20&amp;J21&amp;J22&amp;J23&amp;J24&amp;J25&amp;J26&amp;J27&amp;J28&amp;J29&amp;"],"</f>
+        <v>['Silver Society','Silver Society.svg','y','Downaging','Ageless Consuming','Forever Youngsters','E-Health','Ambient Assisted Living','Slow Culture','Diversity','Liquid Youth','Silver Potentials','Healthness','Universal Design',],</v>
       </c>
       <c r="K30" t="str">
-        <f t="shared" si="0"/>
-        <v>['Mobilität','konn.png','24/7 Gesellschaft','Carsharing','Autonomes Fahren','Third Places','Power of Place','Wearables','Langsamverkehr','E-Mobility','Bike-Boom','Unterwegsmärkte','Mobile Commerce','Mixed Mobility','End-to-End-Tourismus',],</v>
+        <f>"["&amp;K1&amp;K2&amp;K3&amp;K4&amp;K5&amp;K6&amp;K7&amp;K8&amp;K9&amp;K10&amp;K11&amp;K12&amp;K13&amp;K14&amp;K15&amp;K16&amp;K17&amp;K18&amp;K19&amp;K20&amp;K21&amp;K22&amp;K23&amp;K24&amp;K25&amp;K26&amp;K27&amp;K28&amp;K29&amp;"],"</f>
+        <v>['Mobilität','Mobilität.svg','m','24/7 Gesellschaft','Carsharing','Autonomes Fahren','Third Places','Power of Place','Wearables','Langsamverkehr','E-Mobility','Bike-Boom','Unterwegsmärkte','Mobile Commerce','Mixed Mobility','End-to-End-Tourismus',],</v>
       </c>
       <c r="L30" t="str">
-        <f t="shared" si="0"/>
-        <v>['Sicherheit','konn.png','Super-Safe-Society','Trust Technology','Transparenz-Märkte','E-Health','Identitätsmanagement','Digital Reputation','Predictive Analytics','Privacy','Cybercrime','Big Data','Industrie 4.0','Flexicurity','Antifragilität','Simplexity',],</v>
+        <f>"["&amp;L1&amp;L2&amp;L3&amp;L4&amp;L5&amp;L6&amp;L7&amp;L8&amp;L9&amp;L10&amp;L11&amp;L12&amp;L13&amp;L14&amp;L15&amp;L16&amp;L17&amp;L18&amp;L19&amp;L20&amp;L21&amp;L22&amp;L23&amp;L24&amp;L25&amp;L26&amp;L27&amp;L28&amp;L29&amp;"],"</f>
+        <v>['Sicherheit','Sicherheit.svg','s','Super-Safe-Society','Trust Technology','Transparenz-Märkte','E-Health','Identitätsmanagement','Digital Reputation','Predictive Analytics','Privacy','Cybercrime','Big Data','Industrie 4.0','Flexicurity','Antifragilität','Simplexity',],</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="str">
         <f>"var data = ["&amp;A30&amp;B30&amp;C30&amp;D30&amp;E30&amp;F30&amp;G30&amp;H30&amp;I30&amp;J30&amp;K30&amp;L30&amp;M30&amp;N30&amp;O30&amp;P30&amp;Q30&amp;"]"</f>
-        <v>var data = [['Wissenskultur','konn.png','Open Science','Informationsdesign','Bildungsbusiness','Massive Open Online Course','Gamification','Predictive Analytics','Talentismus','Open Innovation','Kollaboration','Sharing Economy','Female Shift','Life-Long-Learning','Tutorial Learning','Creativiteens','Neugiermanagement',],['Konnektivität','konn.png','Augmented Reality','E-Commerce','Crowd Funding','FinTech','Industrie 4.0','Big Data','Cybercrime','Privacy','Predictive Analytics','Selftracking','E-Health','Me-Cloud','Open Innovation','Pop-up Money','Swapping','Smart Devices','Internet der Dinge','Social Networks',],['Urbanisierung','konn.png','Bevölkerungswachstum','Third Places','Collaborative Living','Urban Manufacturing','Urban Mining','Urban Farming','E-Mobility','Bike Boom','Megacities','Global Cities','Landflucht','Schrumpfende Städte','Smart Cities',],['Neo-Ökologie','konn.png','Nachhaltigkeitsgesellschaft','Post-Carbon-Gesellschaft','Bio-Boom','Gutbürger','Slow Culture','Maker Movement','Sharing Economy','Postwachstumsökonomie','Social Business','Fair Trade','Swapping','Zero Waste','Green Tech','Urban Farming','E-Mobility','Circular Economy',],['Globalisierung','konn.png','Glokalisierung','Multipolare Weltordnung','Cybercrime','On-demand Business','Near-shoring','Schattenökonomie','Pop-up Money','Fair Trade','Social Business','Postwachstumsökonomie','Womanomics','Rising Africa','Weltmacht China','Global Cities','Migration',],['Individualisierung','konn.png','Single-Gesellschaft','Lebensqualität','Selftracking','Identitätsmanagement','Me-Cloud','Small-World-Networks','Maker Movement','Diversity','Liquid Youth','Multigrafie','Tutorial Learning','Regenbogenfamilien','Wir-Kultur',],['Gesundheit','konn.png','Sportivity','Detoxing','Komplementärmedizin','Lebensqualität','Selftracking','E-Health','Ambient Assisted Living','Slow Culture','Work-Life-Blending','Corporate Health','Healthness','Foodies','Lebensenergie','Achtsamkeit',],['New Work','konn.png','Work-Design','Outsourcing-Gesellschaft','Start-up-Culture','Slash-Slash-Biografien','Permanent Beta','Silver Potentials','Corporate Health','Work-Life Blending','Diversity','Female Shift','Womanomics','Co-Working','Service-Ökonomie','Social Business','Kollaboration','Open Innovation','Talentismus','On-demand Business','Flexicurity','Antifragilität','Urban Manufacturing','Power of Place','Kreativökonomie',],['Gender Shift','konn.png','Super Daddys','Alpha Softies','Sexdesign','Proll-Professionals','Work-Life-Blending','Diversity','Female Shift','Womanomics','Tiger Woman','Regenbogenfamilien','Neue Mütter','Phasenfamilien',],['Silver Society','konn.png','Downaging','Ageless Consuming','Forever Youngsters','E-Health','Ambient Assisted Living','Slow Culture','Diversity','Liquid Youth','Silver Potentials','Healthness','Universal Design',],['Mobilität','konn.png','24/7 Gesellschaft','Carsharing','Autonomes Fahren','Third Places','Power of Place','Wearables','Langsamverkehr','E-Mobility','Bike-Boom','Unterwegsmärkte','Mobile Commerce','Mixed Mobility','End-to-End-Tourismus',],['Sicherheit','konn.png','Super-Safe-Society','Trust Technology','Transparenz-Märkte','E-Health','Identitätsmanagement','Digital Reputation','Predictive Analytics','Privacy','Cybercrime','Big Data','Industrie 4.0','Flexicurity','Antifragilität','Simplexity',],]</v>
+        <v>var data = [['Wissenskultur','Wissenskultur.svg','w','Open Science','Informationsdesign','Bildungsbusiness','Massive Open Online Course','Gamification','Predictive Analytics','Talentismus','Open Innovation','Kollaboration','Sharing Economy','Female Shift','Life-Long-Learning','Tutorial Learning','Creativiteens','Neugiermanagement',],['Konnektivität','Konnektivität.svg','k','Augmented Reality','E-Commerce','Crowd Funding','FinTech','Industrie 4.0','Big Data','Cybercrime','Privacy','Predictive Analytics','Selftracking','E-Health','Me-Cloud','Open Innovation','Pop-up Money','Swapping','Smart Devices','Internet der Dinge','Social Networks',],['Urbanisierung','Urbanisierung.svg','u','Bevölkerungswachstum','Third Places','Collaborative Living','Urban Manufacturing','Urban Mining','Urban Farming','E-Mobility','Bike Boom','Megacities','Global Cities','Landflucht','Schrumpfende Städte','Smart Cities',],['Neo-Ökologie','Neo-Ökologie.svg','ö','Nachhaltigkeitsgesellschaft','Post-Carbon-Gesellschaft','Bio-Boom','Gutbürger','Slow Culture','Maker Movement','Sharing Economy','Postwachstumsökonomie','Social Business','Fair Trade','Swapping','Zero Waste','Green Tech','Urban Farming','E-Mobility','Circular Economy',],['Globalisierung','Globalisierung.svg','q','Glokalisierung','Multipolare Weltordnung','Cybercrime','On-demand Business','Near-shoring','Schattenökonomie','Pop-up Money','Fair Trade','Social Business','Postwachstumsökonomie','Womanomics','Rising Africa','Weltmacht China','Global Cities','Migration',],['Individualisierung','Individualisierung.svg','i','Single-Gesellschaft','Lebensqualität','Selftracking','Identitätsmanagement','Me-Cloud','Small-World-Networks','Maker Movement','Diversity','Liquid Youth','Multigrafie','Tutorial Learning','Regenbogenfamilien','Wir-Kultur',],['Gesundheit','Gesundheit.svg','g','Sportivity','Detoxing','Komplementärmedizin','Lebensqualität','Selftracking','E-Health','Ambient Assisted Living','Slow Culture','Work-Life-Blending','Corporate Health','Healthness','Foodies','Lebensenergie','Achtsamkeit',],['New Work','New Work.svg','n','Work-Design','Outsourcing-Gesellschaft','Start-up-Culture','Slash-Slash-Biografien','Permanent Beta','Silver Potentials','Corporate Health','Work-Life Blending','Diversity','Female Shift','Womanomics','Co-Working','Service-Ökonomie','Social Business','Kollaboration','Open Innovation','Talentismus','On-demand Business','Flexicurity','Antifragilität','Urban Manufacturing','Power of Place','Kreativökonomie',],['Gender Shift','Gender Shift.svg','t','Super Daddys','Alpha Softies','Sexdesign','Proll-Professionals','Work-Life-Blending','Diversity','Female Shift','Womanomics','Tiger Woman','Regenbogenfamilien','Neue Mütter','Phasenfamilien',],['Silver Society','Silver Society.svg','y','Downaging','Ageless Consuming','Forever Youngsters','E-Health','Ambient Assisted Living','Slow Culture','Diversity','Liquid Youth','Silver Potentials','Healthness','Universal Design',],['Mobilität','Mobilität.svg','m','24/7 Gesellschaft','Carsharing','Autonomes Fahren','Third Places','Power of Place','Wearables','Langsamverkehr','E-Mobility','Bike-Boom','Unterwegsmärkte','Mobile Commerce','Mixed Mobility','End-to-End-Tourismus',],['Sicherheit','Sicherheit.svg','s','Super-Safe-Society','Trust Technology','Transparenz-Märkte','E-Health','Identitätsmanagement','Digital Reputation','Predictive Analytics','Privacy','Cybercrime','Big Data','Industrie 4.0','Flexicurity','Antifragilität','Simplexity',],]</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added sounds and improved usability
</commit_message>
<xml_diff>
--- a/trends.xlsx
+++ b/trends.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mmi/workspaces/shub/symbioticon-2019-slot-machine/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDD92C20-BE8B-3C42-AB2A-9D45E0C9515E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3AB4E51-FB01-A249-8264-73B2AEDD5AF2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="31260" windowHeight="20540" activeTab="1" xr2:uid="{B6AAB51A-975A-FF42-AF23-E449566C1E86}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="31260" windowHeight="20540" xr2:uid="{B6AAB51A-975A-FF42-AF23-E449566C1E86}"/>
   </bookViews>
   <sheets>
     <sheet name="trends" sheetId="1" r:id="rId1"/>
@@ -458,9 +458,6 @@
     <t>Mobilität.svg</t>
   </si>
   <si>
-    <t>Neo-Ökologie.svg</t>
-  </si>
-  <si>
     <t>New Work.svg</t>
   </si>
   <si>
@@ -510,6 +507,9 @@
   </si>
   <si>
     <t>t</t>
+  </si>
+  <si>
+    <t>Neo-Oekologie.svg</t>
   </si>
 </sst>
 </file>
@@ -863,8 +863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC721A76-31B5-5942-83B2-FF5724A5D504}">
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -914,16 +914,16 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B2" t="s">
         <v>135</v>
       </c>
       <c r="C2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D2" t="s">
-        <v>141</v>
+        <v>158</v>
       </c>
       <c r="E2" t="s">
         <v>138</v>
@@ -935,57 +935,57 @@
         <v>137</v>
       </c>
       <c r="H2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I2" t="s">
         <v>136</v>
       </c>
       <c r="J2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K2" t="s">
         <v>140</v>
       </c>
       <c r="L2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B3" t="s">
         <v>147</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>148</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>153</v>
+      </c>
+      <c r="E3" t="s">
+        <v>156</v>
+      </c>
+      <c r="F3" t="s">
+        <v>151</v>
+      </c>
+      <c r="G3" t="s">
+        <v>152</v>
+      </c>
+      <c r="H3" t="s">
         <v>149</v>
       </c>
-      <c r="D3" t="s">
+      <c r="I3" t="s">
+        <v>157</v>
+      </c>
+      <c r="J3" t="s">
+        <v>150</v>
+      </c>
+      <c r="K3" t="s">
+        <v>155</v>
+      </c>
+      <c r="L3" t="s">
         <v>154</v>
-      </c>
-      <c r="E3" t="s">
-        <v>157</v>
-      </c>
-      <c r="F3" t="s">
-        <v>152</v>
-      </c>
-      <c r="G3" t="s">
-        <v>153</v>
-      </c>
-      <c r="H3" t="s">
-        <v>150</v>
-      </c>
-      <c r="I3" t="s">
-        <v>158</v>
-      </c>
-      <c r="J3" t="s">
-        <v>151</v>
-      </c>
-      <c r="K3" t="s">
-        <v>156</v>
-      </c>
-      <c r="L3" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -1574,7 +1574,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{500DDF2F-334E-8A4E-AA45-571C0E2C5A60}">
   <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
@@ -1661,7 +1661,7 @@
       </c>
       <c r="D2" t="str">
         <f>IF(ISBLANK(trends!D2),"","'"&amp;trends!D2&amp;"',")</f>
-        <v>'Neo-Ökologie.svg',</v>
+        <v>'Neo-Oekologie.svg',</v>
       </c>
       <c r="E2" t="str">
         <f>IF(ISBLANK(trends!E2),"","'"&amp;trends!E2&amp;"',")</f>
@@ -3496,58 +3496,58 @@
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" t="str">
-        <f>"["&amp;A1&amp;A2&amp;A3&amp;A4&amp;A5&amp;A6&amp;A7&amp;A8&amp;A9&amp;A10&amp;A11&amp;A12&amp;A13&amp;A14&amp;A15&amp;A16&amp;A17&amp;A18&amp;A19&amp;A20&amp;A21&amp;A22&amp;A23&amp;A24&amp;A25&amp;A26&amp;A27&amp;A28&amp;A29&amp;"],"</f>
+        <f t="shared" ref="A30:L30" si="0">"["&amp;A1&amp;A2&amp;A3&amp;A4&amp;A5&amp;A6&amp;A7&amp;A8&amp;A9&amp;A10&amp;A11&amp;A12&amp;A13&amp;A14&amp;A15&amp;A16&amp;A17&amp;A18&amp;A19&amp;A20&amp;A21&amp;A22&amp;A23&amp;A24&amp;A25&amp;A26&amp;A27&amp;A28&amp;A29&amp;"],"</f>
         <v>['Wissenskultur','Wissenskultur.svg','w','Open Science','Informationsdesign','Bildungsbusiness','Massive Open Online Course','Gamification','Predictive Analytics','Talentismus','Open Innovation','Kollaboration','Sharing Economy','Female Shift','Life-Long-Learning','Tutorial Learning','Creativiteens','Neugiermanagement',],</v>
       </c>
       <c r="B30" t="str">
-        <f>"["&amp;B1&amp;B2&amp;B3&amp;B4&amp;B5&amp;B6&amp;B7&amp;B8&amp;B9&amp;B10&amp;B11&amp;B12&amp;B13&amp;B14&amp;B15&amp;B16&amp;B17&amp;B18&amp;B19&amp;B20&amp;B21&amp;B22&amp;B23&amp;B24&amp;B25&amp;B26&amp;B27&amp;B28&amp;B29&amp;"],"</f>
+        <f t="shared" si="0"/>
         <v>['Konnektivität','Konnektivität.svg','k','Augmented Reality','E-Commerce','Crowd Funding','FinTech','Industrie 4.0','Big Data','Cybercrime','Privacy','Predictive Analytics','Selftracking','E-Health','Me-Cloud','Open Innovation','Pop-up Money','Swapping','Smart Devices','Internet der Dinge','Social Networks',],</v>
       </c>
       <c r="C30" t="str">
-        <f>"["&amp;C1&amp;C2&amp;C3&amp;C4&amp;C5&amp;C6&amp;C7&amp;C8&amp;C9&amp;C10&amp;C11&amp;C12&amp;C13&amp;C14&amp;C15&amp;C16&amp;C17&amp;C18&amp;C19&amp;C20&amp;C21&amp;C22&amp;C23&amp;C24&amp;C25&amp;C26&amp;C27&amp;C28&amp;C29&amp;"],"</f>
+        <f t="shared" si="0"/>
         <v>['Urbanisierung','Urbanisierung.svg','u','Bevölkerungswachstum','Third Places','Collaborative Living','Urban Manufacturing','Urban Mining','Urban Farming','E-Mobility','Bike Boom','Megacities','Global Cities','Landflucht','Schrumpfende Städte','Smart Cities',],</v>
       </c>
       <c r="D30" t="str">
-        <f>"["&amp;D1&amp;D2&amp;D3&amp;D4&amp;D5&amp;D6&amp;D7&amp;D8&amp;D9&amp;D10&amp;D11&amp;D12&amp;D13&amp;D14&amp;D15&amp;D16&amp;D17&amp;D18&amp;D19&amp;D20&amp;D21&amp;D22&amp;D23&amp;D24&amp;D25&amp;D26&amp;D27&amp;D28&amp;D29&amp;"],"</f>
-        <v>['Neo-Ökologie','Neo-Ökologie.svg','ö','Nachhaltigkeitsgesellschaft','Post-Carbon-Gesellschaft','Bio-Boom','Gutbürger','Slow Culture','Maker Movement','Sharing Economy','Postwachstumsökonomie','Social Business','Fair Trade','Swapping','Zero Waste','Green Tech','Urban Farming','E-Mobility','Circular Economy',],</v>
+        <f t="shared" si="0"/>
+        <v>['Neo-Ökologie','Neo-Oekologie.svg','ö','Nachhaltigkeitsgesellschaft','Post-Carbon-Gesellschaft','Bio-Boom','Gutbürger','Slow Culture','Maker Movement','Sharing Economy','Postwachstumsökonomie','Social Business','Fair Trade','Swapping','Zero Waste','Green Tech','Urban Farming','E-Mobility','Circular Economy',],</v>
       </c>
       <c r="E30" t="str">
-        <f>"["&amp;E1&amp;E2&amp;E3&amp;E4&amp;E5&amp;E6&amp;E7&amp;E8&amp;E9&amp;E10&amp;E11&amp;E12&amp;E13&amp;E14&amp;E15&amp;E16&amp;E17&amp;E18&amp;E19&amp;E20&amp;E21&amp;E22&amp;E23&amp;E24&amp;E25&amp;E26&amp;E27&amp;E28&amp;E29&amp;"],"</f>
+        <f t="shared" si="0"/>
         <v>['Globalisierung','Globalisierung.svg','q','Glokalisierung','Multipolare Weltordnung','Cybercrime','On-demand Business','Near-shoring','Schattenökonomie','Pop-up Money','Fair Trade','Social Business','Postwachstumsökonomie','Womanomics','Rising Africa','Weltmacht China','Global Cities','Migration',],</v>
       </c>
       <c r="F30" t="str">
-        <f>"["&amp;F1&amp;F2&amp;F3&amp;F4&amp;F5&amp;F6&amp;F7&amp;F8&amp;F9&amp;F10&amp;F11&amp;F12&amp;F13&amp;F14&amp;F15&amp;F16&amp;F17&amp;F18&amp;F19&amp;F20&amp;F21&amp;F22&amp;F23&amp;F24&amp;F25&amp;F26&amp;F27&amp;F28&amp;F29&amp;"],"</f>
+        <f t="shared" si="0"/>
         <v>['Individualisierung','Individualisierung.svg','i','Single-Gesellschaft','Lebensqualität','Selftracking','Identitätsmanagement','Me-Cloud','Small-World-Networks','Maker Movement','Diversity','Liquid Youth','Multigrafie','Tutorial Learning','Regenbogenfamilien','Wir-Kultur',],</v>
       </c>
       <c r="G30" t="str">
-        <f>"["&amp;G1&amp;G2&amp;G3&amp;G4&amp;G5&amp;G6&amp;G7&amp;G8&amp;G9&amp;G10&amp;G11&amp;G12&amp;G13&amp;G14&amp;G15&amp;G16&amp;G17&amp;G18&amp;G19&amp;G20&amp;G21&amp;G22&amp;G23&amp;G24&amp;G25&amp;G26&amp;G27&amp;G28&amp;G29&amp;"],"</f>
+        <f t="shared" si="0"/>
         <v>['Gesundheit','Gesundheit.svg','g','Sportivity','Detoxing','Komplementärmedizin','Lebensqualität','Selftracking','E-Health','Ambient Assisted Living','Slow Culture','Work-Life-Blending','Corporate Health','Healthness','Foodies','Lebensenergie','Achtsamkeit',],</v>
       </c>
       <c r="H30" t="str">
-        <f>"["&amp;H1&amp;H2&amp;H3&amp;H4&amp;H5&amp;H6&amp;H7&amp;H8&amp;H9&amp;H10&amp;H11&amp;H12&amp;H13&amp;H14&amp;H15&amp;H16&amp;H17&amp;H18&amp;H19&amp;H20&amp;H21&amp;H22&amp;H23&amp;H24&amp;H25&amp;H26&amp;H27&amp;H28&amp;H29&amp;"],"</f>
+        <f t="shared" si="0"/>
         <v>['New Work','New Work.svg','n','Work-Design','Outsourcing-Gesellschaft','Start-up-Culture','Slash-Slash-Biografien','Permanent Beta','Silver Potentials','Corporate Health','Work-Life Blending','Diversity','Female Shift','Womanomics','Co-Working','Service-Ökonomie','Social Business','Kollaboration','Open Innovation','Talentismus','On-demand Business','Flexicurity','Antifragilität','Urban Manufacturing','Power of Place','Kreativökonomie',],</v>
       </c>
       <c r="I30" t="str">
-        <f>"["&amp;I1&amp;I2&amp;I3&amp;I4&amp;I5&amp;I6&amp;I7&amp;I8&amp;I9&amp;I10&amp;I11&amp;I12&amp;I13&amp;I14&amp;I15&amp;I16&amp;I17&amp;I18&amp;I19&amp;I20&amp;I21&amp;I22&amp;I23&amp;I24&amp;I25&amp;I26&amp;I27&amp;I28&amp;I29&amp;"],"</f>
+        <f t="shared" si="0"/>
         <v>['Gender Shift','Gender Shift.svg','t','Super Daddys','Alpha Softies','Sexdesign','Proll-Professionals','Work-Life-Blending','Diversity','Female Shift','Womanomics','Tiger Woman','Regenbogenfamilien','Neue Mütter','Phasenfamilien',],</v>
       </c>
       <c r="J30" t="str">
-        <f>"["&amp;J1&amp;J2&amp;J3&amp;J4&amp;J5&amp;J6&amp;J7&amp;J8&amp;J9&amp;J10&amp;J11&amp;J12&amp;J13&amp;J14&amp;J15&amp;J16&amp;J17&amp;J18&amp;J19&amp;J20&amp;J21&amp;J22&amp;J23&amp;J24&amp;J25&amp;J26&amp;J27&amp;J28&amp;J29&amp;"],"</f>
+        <f t="shared" si="0"/>
         <v>['Silver Society','Silver Society.svg','y','Downaging','Ageless Consuming','Forever Youngsters','E-Health','Ambient Assisted Living','Slow Culture','Diversity','Liquid Youth','Silver Potentials','Healthness','Universal Design',],</v>
       </c>
       <c r="K30" t="str">
-        <f>"["&amp;K1&amp;K2&amp;K3&amp;K4&amp;K5&amp;K6&amp;K7&amp;K8&amp;K9&amp;K10&amp;K11&amp;K12&amp;K13&amp;K14&amp;K15&amp;K16&amp;K17&amp;K18&amp;K19&amp;K20&amp;K21&amp;K22&amp;K23&amp;K24&amp;K25&amp;K26&amp;K27&amp;K28&amp;K29&amp;"],"</f>
+        <f t="shared" si="0"/>
         <v>['Mobilität','Mobilität.svg','m','24/7 Gesellschaft','Carsharing','Autonomes Fahren','Third Places','Power of Place','Wearables','Langsamverkehr','E-Mobility','Bike-Boom','Unterwegsmärkte','Mobile Commerce','Mixed Mobility','End-to-End-Tourismus',],</v>
       </c>
       <c r="L30" t="str">
-        <f>"["&amp;L1&amp;L2&amp;L3&amp;L4&amp;L5&amp;L6&amp;L7&amp;L8&amp;L9&amp;L10&amp;L11&amp;L12&amp;L13&amp;L14&amp;L15&amp;L16&amp;L17&amp;L18&amp;L19&amp;L20&amp;L21&amp;L22&amp;L23&amp;L24&amp;L25&amp;L26&amp;L27&amp;L28&amp;L29&amp;"],"</f>
+        <f t="shared" si="0"/>
         <v>['Sicherheit','Sicherheit.svg','s','Super-Safe-Society','Trust Technology','Transparenz-Märkte','E-Health','Identitätsmanagement','Digital Reputation','Predictive Analytics','Privacy','Cybercrime','Big Data','Industrie 4.0','Flexicurity','Antifragilität','Simplexity',],</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="str">
         <f>"var data = ["&amp;A30&amp;B30&amp;C30&amp;D30&amp;E30&amp;F30&amp;G30&amp;H30&amp;I30&amp;J30&amp;K30&amp;L30&amp;M30&amp;N30&amp;O30&amp;P30&amp;Q30&amp;"]"</f>
-        <v>var data = [['Wissenskultur','Wissenskultur.svg','w','Open Science','Informationsdesign','Bildungsbusiness','Massive Open Online Course','Gamification','Predictive Analytics','Talentismus','Open Innovation','Kollaboration','Sharing Economy','Female Shift','Life-Long-Learning','Tutorial Learning','Creativiteens','Neugiermanagement',],['Konnektivität','Konnektivität.svg','k','Augmented Reality','E-Commerce','Crowd Funding','FinTech','Industrie 4.0','Big Data','Cybercrime','Privacy','Predictive Analytics','Selftracking','E-Health','Me-Cloud','Open Innovation','Pop-up Money','Swapping','Smart Devices','Internet der Dinge','Social Networks',],['Urbanisierung','Urbanisierung.svg','u','Bevölkerungswachstum','Third Places','Collaborative Living','Urban Manufacturing','Urban Mining','Urban Farming','E-Mobility','Bike Boom','Megacities','Global Cities','Landflucht','Schrumpfende Städte','Smart Cities',],['Neo-Ökologie','Neo-Ökologie.svg','ö','Nachhaltigkeitsgesellschaft','Post-Carbon-Gesellschaft','Bio-Boom','Gutbürger','Slow Culture','Maker Movement','Sharing Economy','Postwachstumsökonomie','Social Business','Fair Trade','Swapping','Zero Waste','Green Tech','Urban Farming','E-Mobility','Circular Economy',],['Globalisierung','Globalisierung.svg','q','Glokalisierung','Multipolare Weltordnung','Cybercrime','On-demand Business','Near-shoring','Schattenökonomie','Pop-up Money','Fair Trade','Social Business','Postwachstumsökonomie','Womanomics','Rising Africa','Weltmacht China','Global Cities','Migration',],['Individualisierung','Individualisierung.svg','i','Single-Gesellschaft','Lebensqualität','Selftracking','Identitätsmanagement','Me-Cloud','Small-World-Networks','Maker Movement','Diversity','Liquid Youth','Multigrafie','Tutorial Learning','Regenbogenfamilien','Wir-Kultur',],['Gesundheit','Gesundheit.svg','g','Sportivity','Detoxing','Komplementärmedizin','Lebensqualität','Selftracking','E-Health','Ambient Assisted Living','Slow Culture','Work-Life-Blending','Corporate Health','Healthness','Foodies','Lebensenergie','Achtsamkeit',],['New Work','New Work.svg','n','Work-Design','Outsourcing-Gesellschaft','Start-up-Culture','Slash-Slash-Biografien','Permanent Beta','Silver Potentials','Corporate Health','Work-Life Blending','Diversity','Female Shift','Womanomics','Co-Working','Service-Ökonomie','Social Business','Kollaboration','Open Innovation','Talentismus','On-demand Business','Flexicurity','Antifragilität','Urban Manufacturing','Power of Place','Kreativökonomie',],['Gender Shift','Gender Shift.svg','t','Super Daddys','Alpha Softies','Sexdesign','Proll-Professionals','Work-Life-Blending','Diversity','Female Shift','Womanomics','Tiger Woman','Regenbogenfamilien','Neue Mütter','Phasenfamilien',],['Silver Society','Silver Society.svg','y','Downaging','Ageless Consuming','Forever Youngsters','E-Health','Ambient Assisted Living','Slow Culture','Diversity','Liquid Youth','Silver Potentials','Healthness','Universal Design',],['Mobilität','Mobilität.svg','m','24/7 Gesellschaft','Carsharing','Autonomes Fahren','Third Places','Power of Place','Wearables','Langsamverkehr','E-Mobility','Bike-Boom','Unterwegsmärkte','Mobile Commerce','Mixed Mobility','End-to-End-Tourismus',],['Sicherheit','Sicherheit.svg','s','Super-Safe-Society','Trust Technology','Transparenz-Märkte','E-Health','Identitätsmanagement','Digital Reputation','Predictive Analytics','Privacy','Cybercrime','Big Data','Industrie 4.0','Flexicurity','Antifragilität','Simplexity',],]</v>
+        <v>var data = [['Wissenskultur','Wissenskultur.svg','w','Open Science','Informationsdesign','Bildungsbusiness','Massive Open Online Course','Gamification','Predictive Analytics','Talentismus','Open Innovation','Kollaboration','Sharing Economy','Female Shift','Life-Long-Learning','Tutorial Learning','Creativiteens','Neugiermanagement',],['Konnektivität','Konnektivität.svg','k','Augmented Reality','E-Commerce','Crowd Funding','FinTech','Industrie 4.0','Big Data','Cybercrime','Privacy','Predictive Analytics','Selftracking','E-Health','Me-Cloud','Open Innovation','Pop-up Money','Swapping','Smart Devices','Internet der Dinge','Social Networks',],['Urbanisierung','Urbanisierung.svg','u','Bevölkerungswachstum','Third Places','Collaborative Living','Urban Manufacturing','Urban Mining','Urban Farming','E-Mobility','Bike Boom','Megacities','Global Cities','Landflucht','Schrumpfende Städte','Smart Cities',],['Neo-Ökologie','Neo-Oekologie.svg','ö','Nachhaltigkeitsgesellschaft','Post-Carbon-Gesellschaft','Bio-Boom','Gutbürger','Slow Culture','Maker Movement','Sharing Economy','Postwachstumsökonomie','Social Business','Fair Trade','Swapping','Zero Waste','Green Tech','Urban Farming','E-Mobility','Circular Economy',],['Globalisierung','Globalisierung.svg','q','Glokalisierung','Multipolare Weltordnung','Cybercrime','On-demand Business','Near-shoring','Schattenökonomie','Pop-up Money','Fair Trade','Social Business','Postwachstumsökonomie','Womanomics','Rising Africa','Weltmacht China','Global Cities','Migration',],['Individualisierung','Individualisierung.svg','i','Single-Gesellschaft','Lebensqualität','Selftracking','Identitätsmanagement','Me-Cloud','Small-World-Networks','Maker Movement','Diversity','Liquid Youth','Multigrafie','Tutorial Learning','Regenbogenfamilien','Wir-Kultur',],['Gesundheit','Gesundheit.svg','g','Sportivity','Detoxing','Komplementärmedizin','Lebensqualität','Selftracking','E-Health','Ambient Assisted Living','Slow Culture','Work-Life-Blending','Corporate Health','Healthness','Foodies','Lebensenergie','Achtsamkeit',],['New Work','New Work.svg','n','Work-Design','Outsourcing-Gesellschaft','Start-up-Culture','Slash-Slash-Biografien','Permanent Beta','Silver Potentials','Corporate Health','Work-Life Blending','Diversity','Female Shift','Womanomics','Co-Working','Service-Ökonomie','Social Business','Kollaboration','Open Innovation','Talentismus','On-demand Business','Flexicurity','Antifragilität','Urban Manufacturing','Power of Place','Kreativökonomie',],['Gender Shift','Gender Shift.svg','t','Super Daddys','Alpha Softies','Sexdesign','Proll-Professionals','Work-Life-Blending','Diversity','Female Shift','Womanomics','Tiger Woman','Regenbogenfamilien','Neue Mütter','Phasenfamilien',],['Silver Society','Silver Society.svg','y','Downaging','Ageless Consuming','Forever Youngsters','E-Health','Ambient Assisted Living','Slow Culture','Diversity','Liquid Youth','Silver Potentials','Healthness','Universal Design',],['Mobilität','Mobilität.svg','m','24/7 Gesellschaft','Carsharing','Autonomes Fahren','Third Places','Power of Place','Wearables','Langsamverkehr','E-Mobility','Bike-Boom','Unterwegsmärkte','Mobile Commerce','Mixed Mobility','End-to-End-Tourismus',],['Sicherheit','Sicherheit.svg','s','Super-Safe-Society','Trust Technology','Transparenz-Märkte','E-Health','Identitätsmanagement','Digital Reputation','Predictive Analytics','Privacy','Cybercrime','Big Data','Industrie 4.0','Flexicurity','Antifragilität','Simplexity',],]</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added maps, some minor issues
</commit_message>
<xml_diff>
--- a/trends.xlsx
+++ b/trends.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mmi/workspaces/shub/symbioticon-2019-slot-machine/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3AB4E51-FB01-A249-8264-73B2AEDD5AF2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09730E0E-8F3B-1046-A9B8-8F9F3C24BAF1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="31260" windowHeight="20540" xr2:uid="{B6AAB51A-975A-FF42-AF23-E449566C1E86}"/>
   </bookViews>
@@ -455,9 +455,6 @@
     <t>Individualisierung.svg</t>
   </si>
   <si>
-    <t>Mobilität.svg</t>
-  </si>
-  <si>
     <t>New Work.svg</t>
   </si>
   <si>
@@ -510,6 +507,9 @@
   </si>
   <si>
     <t>Neo-Oekologie.svg</t>
+  </si>
+  <si>
+    <t>Mobilitaet.svg</t>
   </si>
 </sst>
 </file>
@@ -864,7 +864,7 @@
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -914,16 +914,16 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B2" t="s">
         <v>135</v>
       </c>
       <c r="C2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E2" t="s">
         <v>138</v>
@@ -935,57 +935,57 @@
         <v>137</v>
       </c>
       <c r="H2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I2" t="s">
         <v>136</v>
       </c>
       <c r="J2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K2" t="s">
-        <v>140</v>
+        <v>158</v>
       </c>
       <c r="L2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B3" t="s">
         <v>146</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>147</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>152</v>
+      </c>
+      <c r="E3" t="s">
+        <v>155</v>
+      </c>
+      <c r="F3" t="s">
+        <v>150</v>
+      </c>
+      <c r="G3" t="s">
+        <v>151</v>
+      </c>
+      <c r="H3" t="s">
         <v>148</v>
       </c>
-      <c r="D3" t="s">
+      <c r="I3" t="s">
+        <v>156</v>
+      </c>
+      <c r="J3" t="s">
+        <v>149</v>
+      </c>
+      <c r="K3" t="s">
+        <v>154</v>
+      </c>
+      <c r="L3" t="s">
         <v>153</v>
-      </c>
-      <c r="E3" t="s">
-        <v>156</v>
-      </c>
-      <c r="F3" t="s">
-        <v>151</v>
-      </c>
-      <c r="G3" t="s">
-        <v>152</v>
-      </c>
-      <c r="H3" t="s">
-        <v>149</v>
-      </c>
-      <c r="I3" t="s">
-        <v>157</v>
-      </c>
-      <c r="J3" t="s">
-        <v>150</v>
-      </c>
-      <c r="K3" t="s">
-        <v>155</v>
-      </c>
-      <c r="L3" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -1575,7 +1575,7 @@
   <dimension ref="A1:P34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M33" sqref="M33"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1689,7 +1689,7 @@
       </c>
       <c r="K2" t="str">
         <f>IF(ISBLANK(trends!K2),"","'"&amp;trends!K2&amp;"',")</f>
-        <v>'Mobilität.svg',</v>
+        <v>'Mobilitaet.svg',</v>
       </c>
       <c r="L2" t="str">
         <f>IF(ISBLANK(trends!L2),"","'"&amp;trends!L2&amp;"',")</f>
@@ -3537,7 +3537,7 @@
       </c>
       <c r="K30" t="str">
         <f t="shared" si="0"/>
-        <v>['Mobilität','Mobilität.svg','m','24/7 Gesellschaft','Carsharing','Autonomes Fahren','Third Places','Power of Place','Wearables','Langsamverkehr','E-Mobility','Bike-Boom','Unterwegsmärkte','Mobile Commerce','Mixed Mobility','End-to-End-Tourismus',],</v>
+        <v>['Mobilität','Mobilitaet.svg','m','24/7 Gesellschaft','Carsharing','Autonomes Fahren','Third Places','Power of Place','Wearables','Langsamverkehr','E-Mobility','Bike-Boom','Unterwegsmärkte','Mobile Commerce','Mixed Mobility','End-to-End-Tourismus',],</v>
       </c>
       <c r="L30" t="str">
         <f t="shared" si="0"/>
@@ -3547,7 +3547,7 @@
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="str">
         <f>"var data = ["&amp;A30&amp;B30&amp;C30&amp;D30&amp;E30&amp;F30&amp;G30&amp;H30&amp;I30&amp;J30&amp;K30&amp;L30&amp;M30&amp;N30&amp;O30&amp;P30&amp;Q30&amp;"]"</f>
-        <v>var data = [['Wissenskultur','Wissenskultur.svg','w','Open Science','Informationsdesign','Bildungsbusiness','Massive Open Online Course','Gamification','Predictive Analytics','Talentismus','Open Innovation','Kollaboration','Sharing Economy','Female Shift','Life-Long-Learning','Tutorial Learning','Creativiteens','Neugiermanagement',],['Konnektivität','Konnektivität.svg','k','Augmented Reality','E-Commerce','Crowd Funding','FinTech','Industrie 4.0','Big Data','Cybercrime','Privacy','Predictive Analytics','Selftracking','E-Health','Me-Cloud','Open Innovation','Pop-up Money','Swapping','Smart Devices','Internet der Dinge','Social Networks',],['Urbanisierung','Urbanisierung.svg','u','Bevölkerungswachstum','Third Places','Collaborative Living','Urban Manufacturing','Urban Mining','Urban Farming','E-Mobility','Bike Boom','Megacities','Global Cities','Landflucht','Schrumpfende Städte','Smart Cities',],['Neo-Ökologie','Neo-Oekologie.svg','ö','Nachhaltigkeitsgesellschaft','Post-Carbon-Gesellschaft','Bio-Boom','Gutbürger','Slow Culture','Maker Movement','Sharing Economy','Postwachstumsökonomie','Social Business','Fair Trade','Swapping','Zero Waste','Green Tech','Urban Farming','E-Mobility','Circular Economy',],['Globalisierung','Globalisierung.svg','q','Glokalisierung','Multipolare Weltordnung','Cybercrime','On-demand Business','Near-shoring','Schattenökonomie','Pop-up Money','Fair Trade','Social Business','Postwachstumsökonomie','Womanomics','Rising Africa','Weltmacht China','Global Cities','Migration',],['Individualisierung','Individualisierung.svg','i','Single-Gesellschaft','Lebensqualität','Selftracking','Identitätsmanagement','Me-Cloud','Small-World-Networks','Maker Movement','Diversity','Liquid Youth','Multigrafie','Tutorial Learning','Regenbogenfamilien','Wir-Kultur',],['Gesundheit','Gesundheit.svg','g','Sportivity','Detoxing','Komplementärmedizin','Lebensqualität','Selftracking','E-Health','Ambient Assisted Living','Slow Culture','Work-Life-Blending','Corporate Health','Healthness','Foodies','Lebensenergie','Achtsamkeit',],['New Work','New Work.svg','n','Work-Design','Outsourcing-Gesellschaft','Start-up-Culture','Slash-Slash-Biografien','Permanent Beta','Silver Potentials','Corporate Health','Work-Life Blending','Diversity','Female Shift','Womanomics','Co-Working','Service-Ökonomie','Social Business','Kollaboration','Open Innovation','Talentismus','On-demand Business','Flexicurity','Antifragilität','Urban Manufacturing','Power of Place','Kreativökonomie',],['Gender Shift','Gender Shift.svg','t','Super Daddys','Alpha Softies','Sexdesign','Proll-Professionals','Work-Life-Blending','Diversity','Female Shift','Womanomics','Tiger Woman','Regenbogenfamilien','Neue Mütter','Phasenfamilien',],['Silver Society','Silver Society.svg','y','Downaging','Ageless Consuming','Forever Youngsters','E-Health','Ambient Assisted Living','Slow Culture','Diversity','Liquid Youth','Silver Potentials','Healthness','Universal Design',],['Mobilität','Mobilität.svg','m','24/7 Gesellschaft','Carsharing','Autonomes Fahren','Third Places','Power of Place','Wearables','Langsamverkehr','E-Mobility','Bike-Boom','Unterwegsmärkte','Mobile Commerce','Mixed Mobility','End-to-End-Tourismus',],['Sicherheit','Sicherheit.svg','s','Super-Safe-Society','Trust Technology','Transparenz-Märkte','E-Health','Identitätsmanagement','Digital Reputation','Predictive Analytics','Privacy','Cybercrime','Big Data','Industrie 4.0','Flexicurity','Antifragilität','Simplexity',],]</v>
+        <v>var data = [['Wissenskultur','Wissenskultur.svg','w','Open Science','Informationsdesign','Bildungsbusiness','Massive Open Online Course','Gamification','Predictive Analytics','Talentismus','Open Innovation','Kollaboration','Sharing Economy','Female Shift','Life-Long-Learning','Tutorial Learning','Creativiteens','Neugiermanagement',],['Konnektivität','Konnektivität.svg','k','Augmented Reality','E-Commerce','Crowd Funding','FinTech','Industrie 4.0','Big Data','Cybercrime','Privacy','Predictive Analytics','Selftracking','E-Health','Me-Cloud','Open Innovation','Pop-up Money','Swapping','Smart Devices','Internet der Dinge','Social Networks',],['Urbanisierung','Urbanisierung.svg','u','Bevölkerungswachstum','Third Places','Collaborative Living','Urban Manufacturing','Urban Mining','Urban Farming','E-Mobility','Bike Boom','Megacities','Global Cities','Landflucht','Schrumpfende Städte','Smart Cities',],['Neo-Ökologie','Neo-Oekologie.svg','ö','Nachhaltigkeitsgesellschaft','Post-Carbon-Gesellschaft','Bio-Boom','Gutbürger','Slow Culture','Maker Movement','Sharing Economy','Postwachstumsökonomie','Social Business','Fair Trade','Swapping','Zero Waste','Green Tech','Urban Farming','E-Mobility','Circular Economy',],['Globalisierung','Globalisierung.svg','q','Glokalisierung','Multipolare Weltordnung','Cybercrime','On-demand Business','Near-shoring','Schattenökonomie','Pop-up Money','Fair Trade','Social Business','Postwachstumsökonomie','Womanomics','Rising Africa','Weltmacht China','Global Cities','Migration',],['Individualisierung','Individualisierung.svg','i','Single-Gesellschaft','Lebensqualität','Selftracking','Identitätsmanagement','Me-Cloud','Small-World-Networks','Maker Movement','Diversity','Liquid Youth','Multigrafie','Tutorial Learning','Regenbogenfamilien','Wir-Kultur',],['Gesundheit','Gesundheit.svg','g','Sportivity','Detoxing','Komplementärmedizin','Lebensqualität','Selftracking','E-Health','Ambient Assisted Living','Slow Culture','Work-Life-Blending','Corporate Health','Healthness','Foodies','Lebensenergie','Achtsamkeit',],['New Work','New Work.svg','n','Work-Design','Outsourcing-Gesellschaft','Start-up-Culture','Slash-Slash-Biografien','Permanent Beta','Silver Potentials','Corporate Health','Work-Life Blending','Diversity','Female Shift','Womanomics','Co-Working','Service-Ökonomie','Social Business','Kollaboration','Open Innovation','Talentismus','On-demand Business','Flexicurity','Antifragilität','Urban Manufacturing','Power of Place','Kreativökonomie',],['Gender Shift','Gender Shift.svg','t','Super Daddys','Alpha Softies','Sexdesign','Proll-Professionals','Work-Life-Blending','Diversity','Female Shift','Womanomics','Tiger Woman','Regenbogenfamilien','Neue Mütter','Phasenfamilien',],['Silver Society','Silver Society.svg','y','Downaging','Ageless Consuming','Forever Youngsters','E-Health','Ambient Assisted Living','Slow Culture','Diversity','Liquid Youth','Silver Potentials','Healthness','Universal Design',],['Mobilität','Mobilitaet.svg','m','24/7 Gesellschaft','Carsharing','Autonomes Fahren','Third Places','Power of Place','Wearables','Langsamverkehr','E-Mobility','Bike-Boom','Unterwegsmärkte','Mobile Commerce','Mixed Mobility','End-to-End-Tourismus',],['Sicherheit','Sicherheit.svg','s','Super-Safe-Society','Trust Technology','Transparenz-Märkte','E-Health','Identitätsmanagement','Digital Reputation','Predictive Analytics','Privacy','Cybercrime','Big Data','Industrie 4.0','Flexicurity','Antifragilität','Simplexity',],]</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rearranged music, added songs
</commit_message>
<xml_diff>
--- a/trends.xlsx
+++ b/trends.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mmi/workspaces/shub/symbioticon-2019-slot-machine/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E988C2C7-3466-FA46-873A-149638418312}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85413C44-2CE9-3945-8295-F688BE84F5DA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="31260" windowHeight="18680" xr2:uid="{B6AAB51A-975A-FF42-AF23-E449566C1E86}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="193">
   <si>
     <t>Wissenskultur</t>
   </si>
@@ -548,9 +548,6 @@
     <t>open knowledge</t>
   </si>
   <si>
-    <t>playfullness</t>
-  </si>
-  <si>
     <t>Dash delivery</t>
   </si>
   <si>
@@ -597,6 +594,24 @@
   </si>
   <si>
     <t>trust technology</t>
+  </si>
+  <si>
+    <t>playfulness</t>
+  </si>
+  <si>
+    <t>jeopardy</t>
+  </si>
+  <si>
+    <t>mexican</t>
+  </si>
+  <si>
+    <t>dickunddoof</t>
+  </si>
+  <si>
+    <t>pat</t>
+  </si>
+  <si>
+    <t>elephant</t>
   </si>
 </sst>
 </file>
@@ -948,10 +963,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC721A76-31B5-5942-83B2-FF5724A5D504}">
-  <dimension ref="A1:L32"/>
+  <dimension ref="A1:P32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -961,7 +976,7 @@
     <col min="9" max="9" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -999,7 +1014,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>42</v>
       </c>
@@ -1037,7 +1052,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>43</v>
       </c>
@@ -1075,45 +1090,48 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>57</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>188</v>
       </c>
       <c r="C4" t="s">
         <v>59</v>
       </c>
       <c r="D4" t="s">
-        <v>57</v>
+        <v>190</v>
       </c>
       <c r="E4" t="s">
         <v>57</v>
       </c>
       <c r="F4" t="s">
-        <v>57</v>
+        <v>191</v>
       </c>
       <c r="G4" t="s">
         <v>58</v>
       </c>
       <c r="H4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="I4" t="s">
-        <v>57</v>
+        <v>192</v>
       </c>
       <c r="J4" t="s">
-        <v>57</v>
+        <v>190</v>
       </c>
       <c r="K4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="L4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+        <v>188</v>
+      </c>
+      <c r="P4" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>165</v>
       </c>
@@ -1150,8 +1168,11 @@
       <c r="L5" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="P5" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>166</v>
       </c>
@@ -1188,8 +1209,11 @@
       <c r="L6" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="P6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>141</v>
       </c>
@@ -1226,8 +1250,11 @@
       <c r="L7" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="P7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>167</v>
       </c>
@@ -1259,13 +1286,16 @@
         <v>126</v>
       </c>
       <c r="K8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L8" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+        <v>180</v>
+      </c>
+      <c r="P8" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>79</v>
       </c>
@@ -1297,13 +1327,16 @@
         <v>127</v>
       </c>
       <c r="K9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="L9" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="P9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>81</v>
       </c>
@@ -1335,13 +1368,16 @@
         <v>128</v>
       </c>
       <c r="K10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="L10" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="P10" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>168</v>
       </c>
@@ -1373,13 +1409,16 @@
         <v>129</v>
       </c>
       <c r="K11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="L11" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="P11" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>156</v>
       </c>
@@ -1411,13 +1450,13 @@
         <v>130</v>
       </c>
       <c r="K12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="L12" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>84</v>
       </c>
@@ -1449,13 +1488,13 @@
         <v>1</v>
       </c>
       <c r="K13" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="L13" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>86</v>
       </c>
@@ -1487,13 +1526,13 @@
         <v>131</v>
       </c>
       <c r="K14" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="L14" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>169</v>
       </c>
@@ -1522,13 +1561,13 @@
         <v>28</v>
       </c>
       <c r="K15" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="L15" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>146</v>
       </c>
@@ -1580,7 +1619,7 @@
         <v>147</v>
       </c>
       <c r="K17" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="L17" t="s">
         <v>89</v>
@@ -1588,7 +1627,7 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>171</v>
+        <v>187</v>
       </c>
       <c r="B18" t="s">
         <v>82</v>
@@ -1655,7 +1694,7 @@
         <v>66</v>
       </c>
       <c r="L20" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
@@ -1692,7 +1731,7 @@
         <v>151</v>
       </c>
       <c r="L22" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
@@ -1706,7 +1745,7 @@
         <v>140</v>
       </c>
       <c r="L23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
@@ -1717,7 +1756,7 @@
         <v>121</v>
       </c>
       <c r="L24" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
@@ -1773,7 +1812,7 @@
   <dimension ref="A1:P39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1983,7 +2022,7 @@
       </c>
       <c r="B4" t="str">
         <f>IF(ISBLANK(trends!B4),"","'"&amp;trends!B4&amp;"',")</f>
-        <v>'elevator',</v>
+        <v>'jeopardy',</v>
       </c>
       <c r="C4" t="str">
         <f>IF(ISBLANK(trends!C4),"","'"&amp;trends!C4&amp;"',")</f>
@@ -1991,7 +2030,7 @@
       </c>
       <c r="D4" t="str">
         <f>IF(ISBLANK(trends!D4),"","'"&amp;trends!D4&amp;"',")</f>
-        <v>'elevator',</v>
+        <v>'dickunddoof',</v>
       </c>
       <c r="E4" t="str">
         <f>IF(ISBLANK(trends!E4),"","'"&amp;trends!E4&amp;"',")</f>
@@ -1999,7 +2038,7 @@
       </c>
       <c r="F4" t="str">
         <f>IF(ISBLANK(trends!F4),"","'"&amp;trends!F4&amp;"',")</f>
-        <v>'elevator',</v>
+        <v>'pat',</v>
       </c>
       <c r="G4" t="str">
         <f>IF(ISBLANK(trends!G4),"","'"&amp;trends!G4&amp;"',")</f>
@@ -2007,23 +2046,23 @@
       </c>
       <c r="H4" t="str">
         <f>IF(ISBLANK(trends!H4),"","'"&amp;trends!H4&amp;"',")</f>
-        <v>'elevator',</v>
+        <v>'java',</v>
       </c>
       <c r="I4" t="str">
         <f>IF(ISBLANK(trends!I4),"","'"&amp;trends!I4&amp;"',")</f>
-        <v>'elevator',</v>
+        <v>'elephant',</v>
       </c>
       <c r="J4" t="str">
         <f>IF(ISBLANK(trends!J4),"","'"&amp;trends!J4&amp;"',")</f>
-        <v>'elevator',</v>
+        <v>'dickunddoof',</v>
       </c>
       <c r="K4" t="str">
         <f>IF(ISBLANK(trends!K4),"","'"&amp;trends!K4&amp;"',")</f>
-        <v>'elevator',</v>
+        <v>'spanish-flea',</v>
       </c>
       <c r="L4" t="str">
         <f>IF(ISBLANK(trends!L4),"","'"&amp;trends!L4&amp;"',")</f>
-        <v>'elevator',</v>
+        <v>'jeopardy',</v>
       </c>
       <c r="M4" t="str">
         <f>IF(ISBLANK(trends!M4),"","'"&amp;trends!M4&amp;"',")</f>
@@ -2039,7 +2078,7 @@
       </c>
       <c r="P4" t="str">
         <f>IF(ISBLANK(trends!P4),"","'"&amp;trends!P4&amp;"',")</f>
-        <v/>
+        <v>'mexican',</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
@@ -2105,7 +2144,7 @@
       </c>
       <c r="P5" t="str">
         <f>IF(ISBLANK(trends!P5),"","'"&amp;trends!P5&amp;"',")</f>
-        <v/>
+        <v>'pat',</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
@@ -2171,7 +2210,7 @@
       </c>
       <c r="P6" t="str">
         <f>IF(ISBLANK(trends!P6),"","'"&amp;trends!P6&amp;"',")</f>
-        <v/>
+        <v>'java',</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
@@ -2237,7 +2276,7 @@
       </c>
       <c r="P7" t="str">
         <f>IF(ISBLANK(trends!P7),"","'"&amp;trends!P7&amp;"',")</f>
-        <v/>
+        <v>'elevator',</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
@@ -2303,7 +2342,7 @@
       </c>
       <c r="P8" t="str">
         <f>IF(ISBLANK(trends!P8),"","'"&amp;trends!P8&amp;"',")</f>
-        <v/>
+        <v>'dickunddoof',</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
@@ -2369,7 +2408,7 @@
       </c>
       <c r="P9" t="str">
         <f>IF(ISBLANK(trends!P9),"","'"&amp;trends!P9&amp;"',")</f>
-        <v/>
+        <v>'spanish-flea',</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
@@ -2435,7 +2474,7 @@
       </c>
       <c r="P10" t="str">
         <f>IF(ISBLANK(trends!P10),"","'"&amp;trends!P10&amp;"',")</f>
-        <v/>
+        <v>'elephant',</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
@@ -2501,7 +2540,7 @@
       </c>
       <c r="P11" t="str">
         <f>IF(ISBLANK(trends!P11),"","'"&amp;trends!P11&amp;"',")</f>
-        <v/>
+        <v>'jeopardy',</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
@@ -2903,7 +2942,7 @@
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" t="str">
         <f>IF(ISBLANK(trends!A18),"","'"&amp;trends!A18&amp;"',")</f>
-        <v>'playfullness',</v>
+        <v>'playfulness',</v>
       </c>
       <c r="B18" t="str">
         <f>IF(ISBLANK(trends!B18),"","'"&amp;trends!B18&amp;"',")</f>
@@ -3945,11 +3984,11 @@
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" t="str">
         <f>"["&amp;A1&amp;A2&amp;A3&amp;A4&amp;A5&amp;A6&amp;A7&amp;A8&amp;A9&amp;A10&amp;A11&amp;A12&amp;A13&amp;A14&amp;A15&amp;A16&amp;A17&amp;A18&amp;A19&amp;A20&amp;A21&amp;A22&amp;A23&amp;A24&amp;A25&amp;A26&amp;A27&amp;A28&amp;A29&amp;A30&amp;A31&amp;A32&amp;A33&amp;A34&amp;"],"</f>
-        <v>['Wissenskultur','Wissenskultur.svg','w','elevator','augmented learning','bildungs-business','co-working','crowd-sourcing','digital creatives','digital literacy','edutainment','health literacy','kollaboration','learning analytics','lifelong learning','open innovation','open knowledge','playfullness','talentismus','24/7 Gesellschaft',],</v>
+        <v>['Wissenskultur','Wissenskultur.svg','w','elevator','augmented learning','bildungs-business','co-working','crowd-sourcing','digital creatives','digital literacy','edutainment','health literacy','kollaboration','learning analytics','lifelong learning','open innovation','open knowledge','playfulness','talentismus','24/7 Gesellschaft',],</v>
       </c>
       <c r="B35" t="str">
         <f t="shared" ref="B35:L35" si="0">"["&amp;B1&amp;B2&amp;B3&amp;B4&amp;B5&amp;B6&amp;B7&amp;B8&amp;B9&amp;B10&amp;B11&amp;B12&amp;B13&amp;B14&amp;B15&amp;B16&amp;B17&amp;B18&amp;B19&amp;B20&amp;B21&amp;B22&amp;B23&amp;B24&amp;B25&amp;B26&amp;B27&amp;B28&amp;B29&amp;B30&amp;B31&amp;B32&amp;B33&amp;B34&amp;"],"</f>
-        <v>['Konnektivität','Konnektivität.svg','k','elevator','3D-Printing','Augmented reality','autonomes Fahren','Big data','Blockchain','business ecosystems','carsharing','crowdsourcing','crypto-currencies','cybercrime','digital creatives','digital health','digital literacy','digital reputation','internet of things','kollaboration','künstliche Intelligenz','learning analytics','omline','omni-channeling','predictive analytics','privacy','real-digital','seamsless mobility','selftracking','smart city','smart devices','social networks',],</v>
+        <v>['Konnektivität','Konnektivität.svg','k','jeopardy','3D-Printing','Augmented reality','autonomes Fahren','Big data','Blockchain','business ecosystems','carsharing','crowdsourcing','crypto-currencies','cybercrime','digital creatives','digital health','digital literacy','digital reputation','internet of things','kollaboration','künstliche Intelligenz','learning analytics','omline','omni-channeling','predictive analytics','privacy','real-digital','seamsless mobility','selftracking','smart city','smart devices','social networks',],</v>
       </c>
       <c r="C35" t="str">
         <f t="shared" si="0"/>
@@ -3957,7 +3996,7 @@
       </c>
       <c r="D35" t="str">
         <f t="shared" si="0"/>
-        <v>['Neo-Ökologie','Neo-Oekologie.svg','ö','elevator','Achtsamkeit','Bio-Boom','Circular Economy','Direct Trade','E-Mobility','Flexitarier','Green Tech','Gutbürger','Lebensqualität','Minimalismus','Post-Carbon-Gesellschaft','Postwachstumsökonomie','Sharing-economy','Sinn-Ökonomie','slow culture','social business','urban farming','zero waste',],</v>
+        <v>['Neo-Ökologie','Neo-Oekologie.svg','ö','dickunddoof','Achtsamkeit','Bio-Boom','Circular Economy','Direct Trade','E-Mobility','Flexitarier','Green Tech','Gutbürger','Lebensqualität','Minimalismus','Post-Carbon-Gesellschaft','Postwachstumsökonomie','Sharing-economy','Sinn-Ökonomie','slow culture','social business','urban farming','zero waste',],</v>
       </c>
       <c r="E35" t="str">
         <f t="shared" si="0"/>
@@ -3965,7 +4004,7 @@
       </c>
       <c r="F35" t="str">
         <f t="shared" si="0"/>
-        <v>['Individualisierung','Individualisierung.svg','i','elevator','achtsamkeit','alltags outsourcing','diversity','do it yourself','hygge','identitätsmanagement','Lebensqualität','LGBTQ','mass customization','Multigrafie','Neo-Tribes','Postdemografie','Resonanzgesellschaft','self balancer','sex-design','Single-Gesellschaft','Wir-Kultur',],</v>
+        <v>['Individualisierung','Individualisierung.svg','i','pat','achtsamkeit','alltags outsourcing','diversity','do it yourself','hygge','identitätsmanagement','Lebensqualität','LGBTQ','mass customization','Multigrafie','Neo-Tribes','Postdemografie','Resonanzgesellschaft','self balancer','sex-design','Single-Gesellschaft','Wir-Kultur',],</v>
       </c>
       <c r="G35" t="str">
         <f t="shared" si="0"/>
@@ -3973,29 +4012,29 @@
       </c>
       <c r="H35" t="str">
         <f t="shared" si="0"/>
-        <v>['New Work','New Work.svg','n','elevator','Blockchain','business ecosystems','co-working','coopetition','corporate health','digital literacy','diversity','gig economy','internet of things','kollaboration','kreativ-ökonomie','open innovation','permanent beta','plattform ökonomie','service ökonomie','social business','start-up culture','talentismus','urban manufacturing','womanomics','work-life-blending',],</v>
+        <v>['New Work','New Work.svg','n','java','Blockchain','business ecosystems','co-working','coopetition','corporate health','digital literacy','diversity','gig economy','internet of things','kollaboration','kreativ-ökonomie','open innovation','permanent beta','plattform ökonomie','service ökonomie','social business','start-up culture','talentismus','urban manufacturing','womanomics','work-life-blending',],</v>
       </c>
       <c r="I35" t="str">
         <f t="shared" si="0"/>
-        <v>['Gender Shift','Gender Shift.svg','t','elevator','Diversity','LGBTQ','new feminism','post-gender-Marketing','progressive parents','proll professionals','sex-design','ungendered lifestyle','womanomics','work-life-Blending',],</v>
+        <v>['Gender Shift','Gender Shift.svg','t','elephant','Diversity','LGBTQ','new feminism','post-gender-Marketing','progressive parents','proll professionals','sex-design','ungendered lifestyle','womanomics','work-life-Blending',],</v>
       </c>
       <c r="J35" t="str">
         <f t="shared" si="0"/>
-        <v>['Silver Society','Silver Society.svg','y','elevator','digital Health','downaging','forever youngster','free ager','Golden Mentor','Lifelong Learning','Post-Demographie','Slow culture','Talentismus','Unruhestand','Universal Design',],</v>
+        <v>['Silver Society','Silver Society.svg','y','dickunddoof','digital Health','downaging','forever youngster','free ager','Golden Mentor','Lifelong Learning','Post-Demographie','Slow culture','Talentismus','Unruhestand','Universal Design',],</v>
       </c>
       <c r="K35" t="str">
         <f t="shared" si="0"/>
-        <v>['Mobilität','Mobilitaet.svg','m','elevator','autonomes Fahren','Bike-Boom','carsharing','Dash delivery','De-Touristification','E-mobility','Globale Migration','mikro-mobilität','moderne Nomaden','Omni-channeling','Seamsless mobility','third places','Unterwegs-märkte',],</v>
+        <v>['Mobilität','Mobilitaet.svg','m','spanish-flea','autonomes Fahren','Bike-Boom','carsharing','Dash delivery','De-Touristification','E-mobility','Globale Migration','mikro-mobilität','moderne Nomaden','Omni-channeling','Seamsless mobility','third places','Unterwegs-märkte',],</v>
       </c>
       <c r="L35" t="str">
         <f t="shared" si="0"/>
-        <v>['Sicherheit','Sicherheit.svg','s','elevator','autonomes Fahren','big data','Blockchain','business Ecosystems','cybercrime','digital health','digital literacy','digital reputation','flexicurity','hygge','identitäts-management','internet of things','predictive analytics','privacy','selftracking','simplexity','smart city','super-safe-society','transparenzmärkte','trust technology',],</v>
+        <v>['Sicherheit','Sicherheit.svg','s','jeopardy','autonomes Fahren','big data','Blockchain','business Ecosystems','cybercrime','digital health','digital literacy','digital reputation','flexicurity','hygge','identitäts-management','internet of things','predictive analytics','privacy','selftracking','simplexity','smart city','super-safe-society','transparenzmärkte','trust technology',],</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" t="str">
         <f>"var data = ["&amp;A35&amp;B35&amp;C35&amp;D35&amp;E35&amp;F35&amp;G35&amp;H35&amp;I35&amp;J35&amp;K35&amp;L35&amp;M35&amp;N35&amp;O35&amp;P35&amp;Q35&amp;"]"</f>
-        <v>var data = [['Wissenskultur','Wissenskultur.svg','w','elevator','augmented learning','bildungs-business','co-working','crowd-sourcing','digital creatives','digital literacy','edutainment','health literacy','kollaboration','learning analytics','lifelong learning','open innovation','open knowledge','playfullness','talentismus','24/7 Gesellschaft',],['Konnektivität','Konnektivität.svg','k','elevator','3D-Printing','Augmented reality','autonomes Fahren','Big data','Blockchain','business ecosystems','carsharing','crowdsourcing','crypto-currencies','cybercrime','digital creatives','digital health','digital literacy','digital reputation','internet of things','kollaboration','künstliche Intelligenz','learning analytics','omline','omni-channeling','predictive analytics','privacy','real-digital','seamsless mobility','selftracking','smart city','smart devices','social networks',],['Urbanisierung','Urbanisierung.svg','u','java','Big Data','Bike-Boom','Condensed Spaces','Co-Living','Global Cities','healing architecture','megacities','micro housing','progressive provinz','rural cities','smart city','third places','urban farming','urban manufacturing',],['Neo-Ökologie','Neo-Oekologie.svg','ö','elevator','Achtsamkeit','Bio-Boom','Circular Economy','Direct Trade','E-Mobility','Flexitarier','Green Tech','Gutbürger','Lebensqualität','Minimalismus','Post-Carbon-Gesellschaft','Postwachstumsökonomie','Sharing-economy','Sinn-Ökonomie','slow culture','social business','urban farming','zero waste',],['Globalisierung','Globalisierung.svg','q','elevator','Bevölkerungswachstum','Direct Trade','generation global','global cities','globale Migration','Glokalisierung','multipolare Weltordnung','Nearshoring','Neo-Nationalismus','Postwachstumsökonomie','social business',],['Individualisierung','Individualisierung.svg','i','elevator','achtsamkeit','alltags outsourcing','diversity','do it yourself','hygge','identitätsmanagement','Lebensqualität','LGBTQ','mass customization','Multigrafie','Neo-Tribes','Postdemografie','Resonanzgesellschaft','self balancer','sex-design','Single-Gesellschaft','Wir-Kultur',],['Gesundheit','Gesundheit.svg','g','spanish-flea','Achtsamkeit','big data','bike-boom','corporate health','detoxing','digital health','Flexitarier','healing architecture','health literacy','healthy hedonims','holistic health','komplementärmedizin','Lebensqualität','Mind-sport','movement culture','preventive health','sportivity','self balancer','self tracking',],['New Work','New Work.svg','n','elevator','Blockchain','business ecosystems','co-working','coopetition','corporate health','digital literacy','diversity','gig economy','internet of things','kollaboration','kreativ-ökonomie','open innovation','permanent beta','plattform ökonomie','service ökonomie','social business','start-up culture','talentismus','urban manufacturing','womanomics','work-life-blending',],['Gender Shift','Gender Shift.svg','t','elevator','Diversity','LGBTQ','new feminism','post-gender-Marketing','progressive parents','proll professionals','sex-design','ungendered lifestyle','womanomics','work-life-Blending',],['Silver Society','Silver Society.svg','y','elevator','digital Health','downaging','forever youngster','free ager','Golden Mentor','Lifelong Learning','Post-Demographie','Slow culture','Talentismus','Unruhestand','Universal Design',],['Mobilität','Mobilitaet.svg','m','elevator','autonomes Fahren','Bike-Boom','carsharing','Dash delivery','De-Touristification','E-mobility','Globale Migration','mikro-mobilität','moderne Nomaden','Omni-channeling','Seamsless mobility','third places','Unterwegs-märkte',],['Sicherheit','Sicherheit.svg','s','elevator','autonomes Fahren','big data','Blockchain','business Ecosystems','cybercrime','digital health','digital literacy','digital reputation','flexicurity','hygge','identitäts-management','internet of things','predictive analytics','privacy','selftracking','simplexity','smart city','super-safe-society','transparenzmärkte','trust technology',],]</v>
+        <v>var data = [['Wissenskultur','Wissenskultur.svg','w','elevator','augmented learning','bildungs-business','co-working','crowd-sourcing','digital creatives','digital literacy','edutainment','health literacy','kollaboration','learning analytics','lifelong learning','open innovation','open knowledge','playfulness','talentismus','24/7 Gesellschaft',],['Konnektivität','Konnektivität.svg','k','jeopardy','3D-Printing','Augmented reality','autonomes Fahren','Big data','Blockchain','business ecosystems','carsharing','crowdsourcing','crypto-currencies','cybercrime','digital creatives','digital health','digital literacy','digital reputation','internet of things','kollaboration','künstliche Intelligenz','learning analytics','omline','omni-channeling','predictive analytics','privacy','real-digital','seamsless mobility','selftracking','smart city','smart devices','social networks',],['Urbanisierung','Urbanisierung.svg','u','java','Big Data','Bike-Boom','Condensed Spaces','Co-Living','Global Cities','healing architecture','megacities','micro housing','progressive provinz','rural cities','smart city','third places','urban farming','urban manufacturing',],['Neo-Ökologie','Neo-Oekologie.svg','ö','dickunddoof','Achtsamkeit','Bio-Boom','Circular Economy','Direct Trade','E-Mobility','Flexitarier','Green Tech','Gutbürger','Lebensqualität','Minimalismus','Post-Carbon-Gesellschaft','Postwachstumsökonomie','Sharing-economy','Sinn-Ökonomie','slow culture','social business','urban farming','zero waste',],['Globalisierung','Globalisierung.svg','q','elevator','Bevölkerungswachstum','Direct Trade','generation global','global cities','globale Migration','Glokalisierung','multipolare Weltordnung','Nearshoring','Neo-Nationalismus','Postwachstumsökonomie','social business',],['Individualisierung','Individualisierung.svg','i','pat','achtsamkeit','alltags outsourcing','diversity','do it yourself','hygge','identitätsmanagement','Lebensqualität','LGBTQ','mass customization','Multigrafie','Neo-Tribes','Postdemografie','Resonanzgesellschaft','self balancer','sex-design','Single-Gesellschaft','Wir-Kultur',],['Gesundheit','Gesundheit.svg','g','spanish-flea','Achtsamkeit','big data','bike-boom','corporate health','detoxing','digital health','Flexitarier','healing architecture','health literacy','healthy hedonims','holistic health','komplementärmedizin','Lebensqualität','Mind-sport','movement culture','preventive health','sportivity','self balancer','self tracking',],['New Work','New Work.svg','n','java','Blockchain','business ecosystems','co-working','coopetition','corporate health','digital literacy','diversity','gig economy','internet of things','kollaboration','kreativ-ökonomie','open innovation','permanent beta','plattform ökonomie','service ökonomie','social business','start-up culture','talentismus','urban manufacturing','womanomics','work-life-blending',],['Gender Shift','Gender Shift.svg','t','elephant','Diversity','LGBTQ','new feminism','post-gender-Marketing','progressive parents','proll professionals','sex-design','ungendered lifestyle','womanomics','work-life-Blending',],['Silver Society','Silver Society.svg','y','dickunddoof','digital Health','downaging','forever youngster','free ager','Golden Mentor','Lifelong Learning','Post-Demographie','Slow culture','Talentismus','Unruhestand','Universal Design',],['Mobilität','Mobilitaet.svg','m','spanish-flea','autonomes Fahren','Bike-Boom','carsharing','Dash delivery','De-Touristification','E-mobility','Globale Migration','mikro-mobilität','moderne Nomaden','Omni-channeling','Seamsless mobility','third places','Unterwegs-märkte',],['Sicherheit','Sicherheit.svg','s','jeopardy','autonomes Fahren','big data','Blockchain','business Ecosystems','cybercrime','digital health','digital literacy','digital reputation','flexicurity','hygge','identitäts-management','internet of things','predictive analytics','privacy','selftracking','simplexity','smart city','super-safe-society','transparenzmärkte','trust technology',],]</v>
       </c>
     </row>
   </sheetData>

</xml_diff>